<commit_message>
more changes based on learnings
</commit_message>
<xml_diff>
--- a/lighterFluid/inputs/lnlArrayMasterSheet.xlsx
+++ b/lighterFluid/inputs/lnlArrayMasterSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eoghanoc\source\repos\lighterFluid\lighterFluid\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E347848-835C-4F73-8966-1FB2959BF479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E231F871-FE35-4D92-BE5D-2075CBB49386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="templateLookup" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2819" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2829" uniqueCount="292">
   <si>
     <t>Flow</t>
   </si>
@@ -2599,10 +2599,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AH101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="R99" sqref="R99"/>
+      <selection pane="bottomLeft" activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2753,6 +2753,9 @@
       <c r="D3" s="7" t="s">
         <v>26</v>
       </c>
+      <c r="F3" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -2768,6 +2771,9 @@
       <c r="D4" t="s">
         <v>28</v>
       </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
       <c r="W4">
         <v>2</v>
       </c>
@@ -6063,6 +6069,9 @@
       <c r="D38" t="s">
         <v>29</v>
       </c>
+      <c r="F38" t="s">
+        <v>32</v>
+      </c>
       <c r="W38">
         <f t="shared" si="3"/>
         <v>2</v>
@@ -7470,6 +7479,9 @@
       <c r="D56" t="s">
         <v>43</v>
       </c>
+      <c r="F56" t="s">
+        <v>32</v>
+      </c>
       <c r="W56">
         <f t="shared" si="3"/>
         <v>2</v>
@@ -8377,6 +8389,9 @@
       <c r="D67" s="7" t="s">
         <v>48</v>
       </c>
+      <c r="F67" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="68" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
@@ -8900,6 +8915,9 @@
       <c r="D75" s="7" t="s">
         <v>64</v>
       </c>
+      <c r="F75" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="76" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
@@ -9099,6 +9117,9 @@
       <c r="D79" s="7" t="s">
         <v>62</v>
       </c>
+      <c r="F79" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="80" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
@@ -9622,6 +9643,9 @@
       <c r="D87" s="7" t="s">
         <v>63</v>
       </c>
+      <c r="F87" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
@@ -9637,6 +9661,9 @@
       <c r="D88" t="s">
         <v>66</v>
       </c>
+      <c r="F88" t="s">
+        <v>32</v>
+      </c>
       <c r="W88">
         <f t="shared" ref="W88" si="33">COUNTA(Y88:AH88)</f>
         <v>2</v>
@@ -10174,6 +10201,9 @@
       </c>
       <c r="D96" t="s">
         <v>67</v>
+      </c>
+      <c r="F96" t="s">
+        <v>32</v>
       </c>
       <c r="W96">
         <f t="shared" ref="W96" si="36">COUNTA(Y96:AH96)</f>
@@ -10400,8 +10430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E78E7DAD-E2E3-41CA-AC6B-36D49F2F3F66}">
   <dimension ref="A1:AN115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F110" sqref="F110"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10473,16 +10503,16 @@
         <v>94</v>
       </c>
       <c r="T1" t="s">
+        <v>271</v>
+      </c>
+      <c r="U1" t="s">
         <v>137</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>140</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>266</v>
-      </c>
-      <c r="W1" t="s">
-        <v>271</v>
       </c>
       <c r="X1" t="s">
         <v>270</v>
@@ -10701,6 +10731,9 @@
       <c r="S5">
         <v>0</v>
       </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
       <c r="AB5" t="b">
         <v>0</v>
       </c>
@@ -10787,6 +10820,9 @@
       <c r="S6">
         <v>1</v>
       </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
       <c r="X6" t="s">
         <v>272</v>
       </c>
@@ -10873,6 +10909,9 @@
       <c r="S7">
         <v>2</v>
       </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
       <c r="X7" t="s">
         <v>272</v>
       </c>
@@ -10980,6 +11019,9 @@
       <c r="S8">
         <v>3</v>
       </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
       <c r="X8" t="s">
         <v>272</v>
       </c>
@@ -11087,6 +11129,9 @@
       <c r="S9">
         <v>4</v>
       </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
       <c r="X9" t="s">
         <v>273</v>
       </c>
@@ -11173,6 +11218,9 @@
       <c r="S10">
         <v>5</v>
       </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
       <c r="X10" t="s">
         <v>273</v>
       </c>
@@ -11280,6 +11328,9 @@
       <c r="S11">
         <v>6</v>
       </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
       <c r="X11" t="s">
         <v>273</v>
       </c>
@@ -11387,6 +11438,9 @@
       <c r="S12">
         <v>7</v>
       </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
       <c r="X12" t="s">
         <v>274</v>
       </c>
@@ -11473,6 +11527,9 @@
       <c r="S13">
         <v>8</v>
       </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
       <c r="X13" t="s">
         <v>274</v>
       </c>
@@ -11580,6 +11637,9 @@
       <c r="S14">
         <v>9</v>
       </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
       <c r="X14" t="s">
         <v>274</v>
       </c>
@@ -11687,7 +11747,10 @@
       <c r="S15">
         <v>10</v>
       </c>
-      <c r="U15" t="s">
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="V15" t="s">
         <v>264</v>
       </c>
       <c r="AB15" t="b">
@@ -11773,6 +11836,9 @@
       <c r="S16">
         <v>11</v>
       </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
       <c r="AB16" t="b">
         <v>0</v>
       </c>
@@ -11856,6 +11922,9 @@
       <c r="S17">
         <v>12</v>
       </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
       <c r="AB17" t="b">
         <v>0</v>
       </c>
@@ -11935,6 +12004,9 @@
       <c r="S18">
         <v>13</v>
       </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
       <c r="AB18" t="b">
         <v>0</v>
       </c>
@@ -12019,7 +12091,10 @@
       <c r="S19">
         <v>14</v>
       </c>
-      <c r="U19" t="s">
+      <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="V19" t="s">
         <v>267</v>
       </c>
       <c r="AB19" t="b">
@@ -12151,6 +12226,9 @@
       <c r="S22">
         <v>20</v>
       </c>
+      <c r="T22">
+        <v>1</v>
+      </c>
       <c r="AB22" t="b">
         <v>0</v>
       </c>
@@ -12237,6 +12315,9 @@
       <c r="S23">
         <v>21</v>
       </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
       <c r="X23" t="s">
         <v>272</v>
       </c>
@@ -12323,6 +12404,9 @@
       <c r="S24">
         <v>22</v>
       </c>
+      <c r="T24">
+        <v>1</v>
+      </c>
       <c r="X24" t="s">
         <v>272</v>
       </c>
@@ -12430,6 +12514,9 @@
       <c r="S25">
         <v>23</v>
       </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
       <c r="X25" t="s">
         <v>272</v>
       </c>
@@ -12537,6 +12624,9 @@
       <c r="S26">
         <v>24</v>
       </c>
+      <c r="T26">
+        <v>1</v>
+      </c>
       <c r="X26" t="s">
         <v>273</v>
       </c>
@@ -12623,6 +12713,9 @@
       <c r="S27">
         <v>25</v>
       </c>
+      <c r="T27">
+        <v>1</v>
+      </c>
       <c r="X27" t="s">
         <v>273</v>
       </c>
@@ -12730,6 +12823,9 @@
       <c r="S28">
         <v>26</v>
       </c>
+      <c r="T28">
+        <v>1</v>
+      </c>
       <c r="X28" t="s">
         <v>273</v>
       </c>
@@ -12837,6 +12933,9 @@
       <c r="S29">
         <v>27</v>
       </c>
+      <c r="T29">
+        <v>1</v>
+      </c>
       <c r="X29" t="s">
         <v>274</v>
       </c>
@@ -12923,6 +13022,9 @@
       <c r="S30">
         <v>28</v>
       </c>
+      <c r="T30">
+        <v>1</v>
+      </c>
       <c r="X30" t="s">
         <v>274</v>
       </c>
@@ -13030,6 +13132,9 @@
       <c r="S31">
         <v>29</v>
       </c>
+      <c r="T31">
+        <v>1</v>
+      </c>
       <c r="X31" t="s">
         <v>274</v>
       </c>
@@ -13137,7 +13242,10 @@
       <c r="S32">
         <v>30</v>
       </c>
-      <c r="U32" t="s">
+      <c r="T32">
+        <v>1</v>
+      </c>
+      <c r="V32" t="s">
         <v>264</v>
       </c>
       <c r="AB32" t="b">
@@ -13223,6 +13331,9 @@
       <c r="S33">
         <v>31</v>
       </c>
+      <c r="T33">
+        <v>1</v>
+      </c>
       <c r="AB33" t="b">
         <v>0</v>
       </c>
@@ -13306,6 +13417,9 @@
       <c r="S34">
         <v>32</v>
       </c>
+      <c r="T34">
+        <v>1</v>
+      </c>
       <c r="AB34" t="b">
         <v>0</v>
       </c>
@@ -13385,6 +13499,9 @@
       <c r="S35">
         <v>33</v>
       </c>
+      <c r="T35">
+        <v>1</v>
+      </c>
       <c r="AB35" t="b">
         <v>0</v>
       </c>
@@ -13469,7 +13586,10 @@
       <c r="S36">
         <v>34</v>
       </c>
-      <c r="U36" t="s">
+      <c r="T36">
+        <v>1</v>
+      </c>
+      <c r="V36" t="s">
         <v>268</v>
       </c>
       <c r="AB36" t="b">
@@ -13601,6 +13721,9 @@
       <c r="S39">
         <v>0</v>
       </c>
+      <c r="T39">
+        <v>1</v>
+      </c>
       <c r="AB39" t="b">
         <v>0</v>
       </c>
@@ -13687,6 +13810,9 @@
       <c r="S40">
         <v>1</v>
       </c>
+      <c r="T40">
+        <v>1</v>
+      </c>
       <c r="X40" t="s">
         <v>275</v>
       </c>
@@ -13773,6 +13899,9 @@
       <c r="S41">
         <v>2</v>
       </c>
+      <c r="T41">
+        <v>1</v>
+      </c>
       <c r="X41" t="s">
         <v>275</v>
       </c>
@@ -13880,6 +14009,9 @@
       <c r="S42">
         <v>3</v>
       </c>
+      <c r="T42">
+        <v>1</v>
+      </c>
       <c r="X42" t="s">
         <v>275</v>
       </c>
@@ -13987,7 +14119,10 @@
       <c r="S43">
         <v>4</v>
       </c>
-      <c r="U43" t="s">
+      <c r="T43">
+        <v>1</v>
+      </c>
+      <c r="V43" t="s">
         <v>264</v>
       </c>
       <c r="AB43" t="b">
@@ -14073,6 +14208,9 @@
       <c r="S44">
         <v>5</v>
       </c>
+      <c r="T44">
+        <v>1</v>
+      </c>
       <c r="AB44" t="b">
         <v>0</v>
       </c>
@@ -14156,6 +14294,9 @@
       <c r="S45">
         <v>6</v>
       </c>
+      <c r="T45">
+        <v>1</v>
+      </c>
       <c r="AB45" t="b">
         <v>0</v>
       </c>
@@ -14235,6 +14376,9 @@
       <c r="S46">
         <v>7</v>
       </c>
+      <c r="T46">
+        <v>1</v>
+      </c>
       <c r="AB46" t="b">
         <v>0</v>
       </c>
@@ -14319,7 +14463,10 @@
       <c r="S47">
         <v>8</v>
       </c>
-      <c r="U47" t="s">
+      <c r="T47">
+        <v>1</v>
+      </c>
+      <c r="V47" t="s">
         <v>267</v>
       </c>
       <c r="AB47" t="b">
@@ -14451,6 +14598,9 @@
       <c r="S50">
         <v>10</v>
       </c>
+      <c r="T50">
+        <v>1</v>
+      </c>
       <c r="AB50" t="b">
         <v>0</v>
       </c>
@@ -14537,6 +14687,9 @@
       <c r="S51">
         <v>11</v>
       </c>
+      <c r="T51">
+        <v>1</v>
+      </c>
       <c r="X51" t="s">
         <v>275</v>
       </c>
@@ -14623,6 +14776,9 @@
       <c r="S52">
         <v>12</v>
       </c>
+      <c r="T52">
+        <v>1</v>
+      </c>
       <c r="X52" t="s">
         <v>275</v>
       </c>
@@ -14730,6 +14886,9 @@
       <c r="S53">
         <v>13</v>
       </c>
+      <c r="T53">
+        <v>1</v>
+      </c>
       <c r="X53" t="s">
         <v>275</v>
       </c>
@@ -14837,7 +14996,10 @@
       <c r="S54">
         <v>14</v>
       </c>
-      <c r="U54" t="s">
+      <c r="T54">
+        <v>1</v>
+      </c>
+      <c r="V54" t="s">
         <v>264</v>
       </c>
       <c r="AB54" t="b">
@@ -14923,6 +15085,9 @@
       <c r="S55">
         <v>15</v>
       </c>
+      <c r="T55">
+        <v>1</v>
+      </c>
       <c r="AB55" t="b">
         <v>0</v>
       </c>
@@ -15006,6 +15171,9 @@
       <c r="S56">
         <v>16</v>
       </c>
+      <c r="T56">
+        <v>1</v>
+      </c>
       <c r="AB56" t="b">
         <v>0</v>
       </c>
@@ -15085,6 +15253,9 @@
       <c r="S57">
         <v>17</v>
       </c>
+      <c r="T57">
+        <v>1</v>
+      </c>
       <c r="AB57" t="b">
         <v>0</v>
       </c>
@@ -15169,7 +15340,10 @@
       <c r="S58">
         <v>18</v>
       </c>
-      <c r="U58" t="s">
+      <c r="T58">
+        <v>1</v>
+      </c>
+      <c r="V58" t="s">
         <v>268</v>
       </c>
       <c r="AB58" t="b">
@@ -15301,6 +15475,9 @@
       <c r="S61">
         <v>20</v>
       </c>
+      <c r="T61">
+        <v>1</v>
+      </c>
       <c r="X61" t="s">
         <v>276</v>
       </c>
@@ -15393,6 +15570,9 @@
       <c r="S62">
         <v>21</v>
       </c>
+      <c r="T62">
+        <v>1</v>
+      </c>
       <c r="X62" t="s">
         <v>276</v>
       </c>
@@ -15482,6 +15662,9 @@
       <c r="S63">
         <v>22</v>
       </c>
+      <c r="T63">
+        <v>1</v>
+      </c>
       <c r="X63" t="s">
         <v>276</v>
       </c>
@@ -15589,6 +15772,9 @@
       <c r="S64">
         <v>23</v>
       </c>
+      <c r="T64">
+        <v>1</v>
+      </c>
       <c r="X64" t="s">
         <v>276</v>
       </c>
@@ -15696,7 +15882,10 @@
       <c r="S65">
         <v>24</v>
       </c>
-      <c r="U65" t="s">
+      <c r="T65">
+        <v>1</v>
+      </c>
+      <c r="V65" t="s">
         <v>264</v>
       </c>
       <c r="AB65" t="b">
@@ -15782,6 +15971,9 @@
       <c r="S66">
         <v>25</v>
       </c>
+      <c r="T66">
+        <v>1</v>
+      </c>
       <c r="AB66" t="b">
         <v>0</v>
       </c>
@@ -15865,6 +16057,9 @@
       <c r="S67">
         <v>26</v>
       </c>
+      <c r="T67">
+        <v>1</v>
+      </c>
       <c r="AB67" t="b">
         <v>0</v>
       </c>
@@ -15944,6 +16139,9 @@
       <c r="S68">
         <v>27</v>
       </c>
+      <c r="T68">
+        <v>1</v>
+      </c>
       <c r="AB68" t="b">
         <v>0</v>
       </c>
@@ -16028,7 +16226,10 @@
       <c r="S69">
         <v>28</v>
       </c>
-      <c r="U69" t="s">
+      <c r="T69">
+        <v>1</v>
+      </c>
+      <c r="V69" t="s">
         <v>267</v>
       </c>
       <c r="AB69" t="b">
@@ -16160,6 +16361,9 @@
       <c r="S72">
         <v>30</v>
       </c>
+      <c r="T72">
+        <v>1</v>
+      </c>
       <c r="X72" t="s">
         <v>276</v>
       </c>
@@ -16252,6 +16456,9 @@
       <c r="S73">
         <v>31</v>
       </c>
+      <c r="T73">
+        <v>1</v>
+      </c>
       <c r="X73" t="s">
         <v>276</v>
       </c>
@@ -16341,6 +16548,9 @@
       <c r="S74">
         <v>32</v>
       </c>
+      <c r="T74">
+        <v>1</v>
+      </c>
       <c r="X74" t="s">
         <v>276</v>
       </c>
@@ -16448,6 +16658,9 @@
       <c r="S75">
         <v>33</v>
       </c>
+      <c r="T75">
+        <v>1</v>
+      </c>
       <c r="X75" t="s">
         <v>276</v>
       </c>
@@ -16555,7 +16768,10 @@
       <c r="S76">
         <v>34</v>
       </c>
-      <c r="U76" t="s">
+      <c r="T76">
+        <v>1</v>
+      </c>
+      <c r="V76" t="s">
         <v>264</v>
       </c>
       <c r="AB76" t="b">
@@ -16641,6 +16857,9 @@
       <c r="S77">
         <v>35</v>
       </c>
+      <c r="T77">
+        <v>1</v>
+      </c>
       <c r="AB77" t="b">
         <v>0</v>
       </c>
@@ -16724,6 +16943,9 @@
       <c r="S78">
         <v>36</v>
       </c>
+      <c r="T78">
+        <v>1</v>
+      </c>
       <c r="AB78" t="b">
         <v>0</v>
       </c>
@@ -16803,6 +17025,9 @@
       <c r="S79">
         <v>37</v>
       </c>
+      <c r="T79">
+        <v>1</v>
+      </c>
       <c r="AB79" t="b">
         <v>0</v>
       </c>
@@ -16887,7 +17112,10 @@
       <c r="S80">
         <v>38</v>
       </c>
-      <c r="U80" t="s">
+      <c r="T80">
+        <v>1</v>
+      </c>
+      <c r="V80" t="s">
         <v>268</v>
       </c>
       <c r="AB80" t="b">
@@ -17016,6 +17244,9 @@
       <c r="S83">
         <v>40</v>
       </c>
+      <c r="T83">
+        <v>1</v>
+      </c>
       <c r="AB83" t="b">
         <v>0</v>
       </c>
@@ -17101,6 +17332,9 @@
       </c>
       <c r="S84">
         <v>41</v>
+      </c>
+      <c r="T84">
+        <v>1</v>
       </c>
       <c r="AB84" t="b">
         <v>0</v>
@@ -17296,7 +17530,7 @@
       <c r="S88">
         <v>200</v>
       </c>
-      <c r="T88">
+      <c r="U88">
         <v>2100</v>
       </c>
       <c r="AB88" t="b">
@@ -17378,7 +17612,7 @@
       <c r="S89">
         <v>201</v>
       </c>
-      <c r="T89">
+      <c r="U89">
         <v>2101</v>
       </c>
       <c r="AB89" t="b">
@@ -17460,7 +17694,7 @@
       <c r="S90">
         <v>202</v>
       </c>
-      <c r="T90">
+      <c r="U90">
         <v>2102</v>
       </c>
       <c r="AB90" t="b">
@@ -17542,7 +17776,7 @@
       <c r="S91">
         <v>203</v>
       </c>
-      <c r="T91">
+      <c r="U91">
         <v>2103</v>
       </c>
       <c r="AB91" t="b">
@@ -17996,7 +18230,7 @@
       <c r="S98">
         <v>400</v>
       </c>
-      <c r="T98">
+      <c r="U98">
         <v>2010</v>
       </c>
       <c r="AB98" t="b">
@@ -18078,7 +18312,7 @@
       <c r="S99">
         <v>401</v>
       </c>
-      <c r="T99">
+      <c r="U99">
         <v>2011</v>
       </c>
       <c r="AB99" t="b">
@@ -18160,7 +18394,7 @@
       <c r="S100">
         <v>402</v>
       </c>
-      <c r="T100">
+      <c r="U100">
         <v>2012</v>
       </c>
       <c r="AB100" t="b">
@@ -18242,7 +18476,7 @@
       <c r="S101">
         <v>403</v>
       </c>
-      <c r="T101">
+      <c r="U101">
         <v>2013</v>
       </c>
       <c r="AB101" t="b">
@@ -18457,7 +18691,7 @@
       <c r="S105">
         <v>500</v>
       </c>
-      <c r="T105">
+      <c r="U105">
         <v>2020</v>
       </c>
       <c r="AB105" t="b">
@@ -18539,7 +18773,7 @@
       <c r="S106">
         <v>501</v>
       </c>
-      <c r="T106">
+      <c r="U106">
         <v>2021</v>
       </c>
       <c r="AB106" t="b">
@@ -18621,7 +18855,7 @@
       <c r="S107">
         <v>502</v>
       </c>
-      <c r="T107">
+      <c r="U107">
         <v>2022</v>
       </c>
       <c r="AB107" t="b">
@@ -18703,7 +18937,7 @@
       <c r="S108">
         <v>503</v>
       </c>
-      <c r="T108">
+      <c r="U108">
         <v>2023</v>
       </c>
       <c r="AB108" t="b">
@@ -18826,7 +19060,7 @@
       <c r="S111">
         <v>600</v>
       </c>
-      <c r="T111">
+      <c r="U111">
         <v>2030</v>
       </c>
       <c r="AB111" t="b">
@@ -18908,7 +19142,7 @@
       <c r="S112">
         <v>601</v>
       </c>
-      <c r="T112">
+      <c r="U112">
         <v>2031</v>
       </c>
       <c r="AB112" t="b">

</xml_diff>

<commit_message>
WHY DOES PRIME HAVE DIFFERENT BYPASS RULES. INT VS STR, DIFF NAME, MAKES CODING AROUND IT PAINFUL
</commit_message>
<xml_diff>
--- a/lighterFluid/inputs/lnlArrayMasterSheet.xlsx
+++ b/lighterFluid/inputs/lnlArrayMasterSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eoghanoc\source\repos\lighterFluid\lighterFluid\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534DB927-017B-4962-A6D5-14FEA5FA24DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B075908B-91DE-4699-8E68-201A72418397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2612,9 +2612,9 @@
   <dimension ref="A1:AJ101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="T5" sqref="T5"/>
+      <selection pane="bottomLeft" activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2868,6 +2868,9 @@
       <c r="S5">
         <v>0</v>
       </c>
+      <c r="T5">
+        <v>-1</v>
+      </c>
       <c r="X5" t="b">
         <v>0</v>
       </c>
@@ -2976,6 +2979,9 @@
       <c r="S6">
         <v>1</v>
       </c>
+      <c r="T6">
+        <v>-1</v>
+      </c>
       <c r="X6" t="b">
         <v>0</v>
       </c>
@@ -3072,6 +3078,9 @@
       <c r="S7">
         <v>2</v>
       </c>
+      <c r="T7">
+        <v>-1</v>
+      </c>
       <c r="X7" t="b">
         <v>0</v>
       </c>
@@ -3180,6 +3189,9 @@
       <c r="S8">
         <v>3</v>
       </c>
+      <c r="T8">
+        <v>-1</v>
+      </c>
       <c r="X8" t="b">
         <v>0</v>
       </c>
@@ -3276,6 +3288,9 @@
       <c r="S9">
         <v>4</v>
       </c>
+      <c r="T9">
+        <v>-1</v>
+      </c>
       <c r="X9" t="b">
         <v>0</v>
       </c>
@@ -3384,6 +3399,9 @@
       <c r="S10">
         <v>5</v>
       </c>
+      <c r="T10">
+        <v>-1</v>
+      </c>
       <c r="X10" t="b">
         <v>0</v>
       </c>
@@ -3480,6 +3498,9 @@
       <c r="S11">
         <v>6</v>
       </c>
+      <c r="T11">
+        <v>-1</v>
+      </c>
       <c r="X11" t="b">
         <v>0</v>
       </c>
@@ -3588,6 +3609,9 @@
       <c r="S12">
         <v>7</v>
       </c>
+      <c r="T12">
+        <v>-1</v>
+      </c>
       <c r="X12" t="b">
         <v>0</v>
       </c>
@@ -3684,6 +3708,9 @@
       <c r="S13">
         <v>8</v>
       </c>
+      <c r="T13">
+        <v>-1</v>
+      </c>
       <c r="X13" t="b">
         <v>0</v>
       </c>
@@ -3792,6 +3819,9 @@
       <c r="S14">
         <v>9</v>
       </c>
+      <c r="T14">
+        <v>-1</v>
+      </c>
       <c r="X14" t="b">
         <v>0</v>
       </c>
@@ -3888,6 +3918,9 @@
       <c r="S15">
         <v>10</v>
       </c>
+      <c r="T15">
+        <v>-1</v>
+      </c>
       <c r="X15" t="b">
         <v>0</v>
       </c>
@@ -3996,6 +4029,9 @@
       <c r="S16">
         <v>11</v>
       </c>
+      <c r="T16">
+        <v>-1</v>
+      </c>
       <c r="X16" t="b">
         <v>0</v>
       </c>
@@ -4092,6 +4128,9 @@
       <c r="S17">
         <v>12</v>
       </c>
+      <c r="T17">
+        <v>-1</v>
+      </c>
       <c r="X17" t="b">
         <v>0</v>
       </c>
@@ -4200,6 +4239,9 @@
       <c r="S18">
         <v>13</v>
       </c>
+      <c r="T18">
+        <v>-1</v>
+      </c>
       <c r="X18" t="b">
         <v>0</v>
       </c>
@@ -4296,6 +4338,9 @@
       <c r="S19">
         <v>14</v>
       </c>
+      <c r="T19">
+        <v>-1</v>
+      </c>
       <c r="X19" t="b">
         <v>0</v>
       </c>
@@ -4404,6 +4449,9 @@
       <c r="S20">
         <v>15</v>
       </c>
+      <c r="T20">
+        <v>-1</v>
+      </c>
       <c r="X20" t="b">
         <v>0</v>
       </c>
@@ -4500,6 +4548,9 @@
       <c r="S21">
         <v>16</v>
       </c>
+      <c r="T21">
+        <v>-1</v>
+      </c>
       <c r="X21" t="b">
         <v>0</v>
       </c>
@@ -4608,6 +4659,9 @@
       <c r="S22">
         <v>17</v>
       </c>
+      <c r="T22">
+        <v>-1</v>
+      </c>
       <c r="X22" t="b">
         <v>0</v>
       </c>
@@ -4704,6 +4758,9 @@
       <c r="S23">
         <v>18</v>
       </c>
+      <c r="T23">
+        <v>-1</v>
+      </c>
       <c r="X23" t="b">
         <v>0</v>
       </c>
@@ -4812,6 +4869,9 @@
       <c r="S24">
         <v>19</v>
       </c>
+      <c r="T24">
+        <v>-1</v>
+      </c>
       <c r="X24" t="b">
         <v>0</v>
       </c>
@@ -4908,6 +4968,9 @@
       <c r="S25">
         <v>20</v>
       </c>
+      <c r="T25">
+        <v>-1</v>
+      </c>
       <c r="X25" t="b">
         <v>0</v>
       </c>
@@ -5016,6 +5079,9 @@
       <c r="S26">
         <v>21</v>
       </c>
+      <c r="T26">
+        <v>-1</v>
+      </c>
       <c r="X26" t="b">
         <v>0</v>
       </c>
@@ -5112,6 +5178,9 @@
       <c r="S27">
         <v>22</v>
       </c>
+      <c r="T27">
+        <v>-1</v>
+      </c>
       <c r="X27" t="b">
         <v>0</v>
       </c>
@@ -5220,6 +5289,9 @@
       <c r="S28">
         <v>23</v>
       </c>
+      <c r="T28">
+        <v>-1</v>
+      </c>
       <c r="X28" t="b">
         <v>0</v>
       </c>
@@ -5316,6 +5388,9 @@
       <c r="S29">
         <v>24</v>
       </c>
+      <c r="T29">
+        <v>-1</v>
+      </c>
       <c r="X29" t="b">
         <v>0</v>
       </c>
@@ -5424,6 +5499,9 @@
       <c r="S30">
         <v>25</v>
       </c>
+      <c r="T30">
+        <v>-1</v>
+      </c>
       <c r="X30" t="b">
         <v>0</v>
       </c>
@@ -5520,6 +5598,9 @@
       <c r="S31">
         <v>26</v>
       </c>
+      <c r="T31">
+        <v>-1</v>
+      </c>
       <c r="X31" t="b">
         <v>0</v>
       </c>
@@ -5628,6 +5709,9 @@
       <c r="S32">
         <v>27</v>
       </c>
+      <c r="T32">
+        <v>-1</v>
+      </c>
       <c r="X32" t="b">
         <v>0</v>
       </c>
@@ -5724,6 +5808,9 @@
       <c r="S33">
         <v>28</v>
       </c>
+      <c r="T33">
+        <v>-1</v>
+      </c>
       <c r="X33" t="b">
         <v>0</v>
       </c>
@@ -5832,6 +5919,9 @@
       <c r="S34">
         <v>29</v>
       </c>
+      <c r="T34">
+        <v>-1</v>
+      </c>
       <c r="X34" t="b">
         <v>0</v>
       </c>
@@ -5928,6 +6018,9 @@
       <c r="S35">
         <v>30</v>
       </c>
+      <c r="T35">
+        <v>-1</v>
+      </c>
       <c r="X35" t="b">
         <v>0</v>
       </c>
@@ -6032,6 +6125,9 @@
       <c r="S36">
         <v>31</v>
       </c>
+      <c r="T36">
+        <v>-1</v>
+      </c>
       <c r="X36" t="b">
         <v>0</v>
       </c>
@@ -6166,6 +6262,9 @@
       <c r="S39">
         <v>35</v>
       </c>
+      <c r="T39">
+        <v>-1</v>
+      </c>
       <c r="W39" t="s">
         <v>144</v>
       </c>
@@ -6252,6 +6351,9 @@
       <c r="S40">
         <v>36</v>
       </c>
+      <c r="T40">
+        <v>-1</v>
+      </c>
       <c r="W40" t="s">
         <v>145</v>
       </c>
@@ -6338,6 +6440,9 @@
       <c r="S41">
         <v>37</v>
       </c>
+      <c r="T41">
+        <v>-1</v>
+      </c>
       <c r="W41" t="s">
         <v>146</v>
       </c>
@@ -6424,6 +6529,9 @@
       <c r="S42">
         <v>38</v>
       </c>
+      <c r="T42">
+        <v>-1</v>
+      </c>
       <c r="W42" t="s">
         <v>141</v>
       </c>
@@ -6510,6 +6618,9 @@
       <c r="S43">
         <v>39</v>
       </c>
+      <c r="T43">
+        <v>-1</v>
+      </c>
       <c r="W43" t="s">
         <v>142</v>
       </c>
@@ -6596,6 +6707,9 @@
       <c r="S44">
         <v>40</v>
       </c>
+      <c r="T44">
+        <v>-1</v>
+      </c>
       <c r="W44" t="s">
         <v>143</v>
       </c>
@@ -6682,6 +6796,9 @@
       <c r="S45">
         <v>41</v>
       </c>
+      <c r="T45">
+        <v>-1</v>
+      </c>
       <c r="W45" t="s">
         <v>187</v>
       </c>
@@ -6768,6 +6885,9 @@
       <c r="S46">
         <v>42</v>
       </c>
+      <c r="T46">
+        <v>-1</v>
+      </c>
       <c r="W46" t="s">
         <v>150</v>
       </c>
@@ -6854,6 +6974,9 @@
       <c r="S47">
         <v>43</v>
       </c>
+      <c r="T47">
+        <v>-1</v>
+      </c>
       <c r="W47" t="s">
         <v>151</v>
       </c>
@@ -6940,6 +7063,9 @@
       <c r="S48">
         <v>44</v>
       </c>
+      <c r="T48">
+        <v>-1</v>
+      </c>
       <c r="W48" t="s">
         <v>152</v>
       </c>
@@ -7026,6 +7152,9 @@
       <c r="S49">
         <v>45</v>
       </c>
+      <c r="T49">
+        <v>-1</v>
+      </c>
       <c r="W49" t="s">
         <v>147</v>
       </c>
@@ -7112,6 +7241,9 @@
       <c r="S50">
         <v>46</v>
       </c>
+      <c r="T50">
+        <v>-1</v>
+      </c>
       <c r="W50" t="s">
         <v>148</v>
       </c>
@@ -7198,6 +7330,9 @@
       <c r="S51">
         <v>47</v>
       </c>
+      <c r="T51">
+        <v>-1</v>
+      </c>
       <c r="W51" t="s">
         <v>149</v>
       </c>
@@ -7284,6 +7419,9 @@
       <c r="S52">
         <v>48</v>
       </c>
+      <c r="T52">
+        <v>-1</v>
+      </c>
       <c r="W52" t="s">
         <v>188</v>
       </c>
@@ -7370,6 +7508,9 @@
       <c r="S53">
         <v>49</v>
       </c>
+      <c r="T53">
+        <v>-1</v>
+      </c>
       <c r="X53" t="b">
         <v>1</v>
       </c>
@@ -7454,6 +7595,9 @@
       <c r="S54">
         <v>50</v>
       </c>
+      <c r="T54">
+        <v>-1</v>
+      </c>
       <c r="X54" t="b">
         <v>0</v>
       </c>
@@ -7575,6 +7719,9 @@
       <c r="S57">
         <v>100</v>
       </c>
+      <c r="T57">
+        <v>-1</v>
+      </c>
       <c r="X57" t="b">
         <v>0</v>
       </c>
@@ -7683,6 +7830,9 @@
       <c r="S58">
         <v>101</v>
       </c>
+      <c r="T58">
+        <v>-1</v>
+      </c>
       <c r="X58" t="b">
         <v>0</v>
       </c>
@@ -7791,6 +7941,9 @@
       <c r="S59">
         <v>102</v>
       </c>
+      <c r="T59">
+        <v>-1</v>
+      </c>
       <c r="X59" t="b">
         <v>0</v>
       </c>
@@ -7899,6 +8052,9 @@
       <c r="S60">
         <v>103</v>
       </c>
+      <c r="T60">
+        <v>-1</v>
+      </c>
       <c r="X60" t="b">
         <v>0</v>
       </c>
@@ -8007,6 +8163,9 @@
       <c r="S61">
         <v>104</v>
       </c>
+      <c r="T61">
+        <v>-1</v>
+      </c>
       <c r="X61" t="b">
         <v>0</v>
       </c>
@@ -8115,6 +8274,9 @@
       <c r="S62">
         <v>105</v>
       </c>
+      <c r="T62">
+        <v>-1</v>
+      </c>
       <c r="X62" t="b">
         <v>0</v>
       </c>
@@ -8223,6 +8385,9 @@
       <c r="S63">
         <v>106</v>
       </c>
+      <c r="T63">
+        <v>-1</v>
+      </c>
       <c r="X63" t="b">
         <v>0</v>
       </c>
@@ -8331,6 +8496,9 @@
       <c r="S64">
         <v>107</v>
       </c>
+      <c r="T64">
+        <v>-1</v>
+      </c>
       <c r="X64" t="b">
         <v>0</v>
       </c>
@@ -8472,6 +8640,9 @@
       <c r="S68">
         <v>200</v>
       </c>
+      <c r="T68">
+        <v>-1</v>
+      </c>
       <c r="U68" t="s">
         <v>294</v>
       </c>
@@ -8558,6 +8729,9 @@
       <c r="S69">
         <v>201</v>
       </c>
+      <c r="T69">
+        <v>-1</v>
+      </c>
       <c r="U69" t="s">
         <v>295</v>
       </c>
@@ -8644,6 +8818,9 @@
       <c r="S70">
         <v>202</v>
       </c>
+      <c r="T70">
+        <v>-1</v>
+      </c>
       <c r="U70" t="s">
         <v>294</v>
       </c>
@@ -8730,6 +8907,9 @@
       <c r="S71">
         <v>203</v>
       </c>
+      <c r="T71">
+        <v>-1</v>
+      </c>
       <c r="U71" t="s">
         <v>294</v>
       </c>
@@ -8816,6 +8996,9 @@
       <c r="S72">
         <v>204</v>
       </c>
+      <c r="T72">
+        <v>-1</v>
+      </c>
       <c r="U72" t="s">
         <v>295</v>
       </c>
@@ -8902,6 +9085,9 @@
       <c r="S73">
         <v>205</v>
       </c>
+      <c r="T73">
+        <v>-1</v>
+      </c>
       <c r="U73" t="s">
         <v>294</v>
       </c>
@@ -9016,6 +9202,9 @@
       <c r="S76">
         <v>300</v>
       </c>
+      <c r="T76">
+        <v>-1</v>
+      </c>
       <c r="U76" t="s">
         <v>294</v>
       </c>
@@ -9107,6 +9296,9 @@
       <c r="S77">
         <v>301</v>
       </c>
+      <c r="T77">
+        <v>-1</v>
+      </c>
       <c r="U77" t="s">
         <v>295</v>
       </c>
@@ -9224,6 +9416,9 @@
       <c r="S80">
         <v>400</v>
       </c>
+      <c r="T80">
+        <v>-1</v>
+      </c>
       <c r="U80" t="s">
         <v>294</v>
       </c>
@@ -9310,6 +9505,9 @@
       <c r="S81">
         <v>401</v>
       </c>
+      <c r="T81">
+        <v>-1</v>
+      </c>
       <c r="U81" t="s">
         <v>295</v>
       </c>
@@ -9396,6 +9594,9 @@
       <c r="S82">
         <v>402</v>
       </c>
+      <c r="T82">
+        <v>-1</v>
+      </c>
       <c r="U82" t="s">
         <v>294</v>
       </c>
@@ -9482,6 +9683,9 @@
       <c r="S83">
         <v>403</v>
       </c>
+      <c r="T83">
+        <v>-1</v>
+      </c>
       <c r="U83" t="s">
         <v>294</v>
       </c>
@@ -9568,6 +9772,9 @@
       <c r="S84">
         <v>404</v>
       </c>
+      <c r="T84">
+        <v>-1</v>
+      </c>
       <c r="U84" t="s">
         <v>295</v>
       </c>
@@ -9654,6 +9861,9 @@
       <c r="S85">
         <v>405</v>
       </c>
+      <c r="T85">
+        <v>-1</v>
+      </c>
       <c r="U85" t="s">
         <v>294</v>
       </c>
@@ -9801,6 +10011,9 @@
       <c r="S89">
         <v>500</v>
       </c>
+      <c r="T89">
+        <v>-1</v>
+      </c>
       <c r="U89" t="s">
         <v>294</v>
       </c>
@@ -9887,6 +10100,9 @@
       <c r="S90">
         <v>501</v>
       </c>
+      <c r="T90">
+        <v>-1</v>
+      </c>
       <c r="U90" t="s">
         <v>295</v>
       </c>
@@ -9973,6 +10189,9 @@
       <c r="S91">
         <v>502</v>
       </c>
+      <c r="T91">
+        <v>-1</v>
+      </c>
       <c r="U91" t="s">
         <v>294</v>
       </c>
@@ -10059,6 +10278,9 @@
       <c r="S92">
         <v>503</v>
       </c>
+      <c r="T92">
+        <v>-1</v>
+      </c>
       <c r="U92" t="s">
         <v>294</v>
       </c>
@@ -10145,6 +10367,9 @@
       <c r="S93">
         <v>504</v>
       </c>
+      <c r="T93">
+        <v>-1</v>
+      </c>
       <c r="U93" t="s">
         <v>295</v>
       </c>
@@ -10231,6 +10456,9 @@
       <c r="S94">
         <v>505</v>
       </c>
+      <c r="T94">
+        <v>-1</v>
+      </c>
       <c r="U94" t="s">
         <v>294</v>
       </c>
@@ -10357,6 +10585,9 @@
       <c r="S97">
         <v>600</v>
       </c>
+      <c r="T97">
+        <v>-1</v>
+      </c>
       <c r="U97" t="s">
         <v>294</v>
       </c>
@@ -10441,6 +10672,9 @@
       </c>
       <c r="S98">
         <v>601</v>
+      </c>
+      <c r="T98">
+        <v>-1</v>
       </c>
       <c r="U98" t="s">
         <v>295</v>
@@ -10514,8 +10748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E78E7DAD-E2E3-41CA-AC6B-36D49F2F3F66}">
   <dimension ref="A1:AO115"/>
   <sheetViews>
-    <sheetView topLeftCell="E79" workbookViewId="0">
-      <selection activeCell="U101" sqref="U101"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="T105" sqref="T105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17624,6 +17858,9 @@
       <c r="S88">
         <v>200</v>
       </c>
+      <c r="T88">
+        <v>-1</v>
+      </c>
       <c r="U88" t="s">
         <v>292</v>
       </c>
@@ -17709,6 +17946,9 @@
       <c r="S89">
         <v>201</v>
       </c>
+      <c r="T89">
+        <v>-1</v>
+      </c>
       <c r="U89" t="s">
         <v>292</v>
       </c>
@@ -17794,6 +18034,9 @@
       <c r="S90">
         <v>202</v>
       </c>
+      <c r="T90">
+        <v>-1</v>
+      </c>
       <c r="U90" t="s">
         <v>292</v>
       </c>
@@ -17878,6 +18121,9 @@
       </c>
       <c r="S91">
         <v>203</v>
+      </c>
+      <c r="T91">
+        <v>-1</v>
       </c>
       <c r="U91" t="s">
         <v>293</v>
@@ -18066,6 +18312,9 @@
       <c r="S94">
         <v>300</v>
       </c>
+      <c r="T94">
+        <v>-1</v>
+      </c>
       <c r="U94" t="s">
         <v>292</v>
       </c>
@@ -18155,6 +18404,9 @@
       </c>
       <c r="S95">
         <v>301</v>
+      </c>
+      <c r="T95">
+        <v>-1</v>
       </c>
       <c r="U95" t="s">
         <v>293</v>
@@ -18346,6 +18598,9 @@
       <c r="S98">
         <v>400</v>
       </c>
+      <c r="T98">
+        <v>-1</v>
+      </c>
       <c r="U98" t="s">
         <v>292</v>
       </c>
@@ -18431,6 +18686,9 @@
       <c r="S99">
         <v>401</v>
       </c>
+      <c r="T99">
+        <v>-1</v>
+      </c>
       <c r="U99" t="s">
         <v>292</v>
       </c>
@@ -18516,6 +18774,9 @@
       <c r="S100">
         <v>402</v>
       </c>
+      <c r="T100">
+        <v>-1</v>
+      </c>
       <c r="U100" t="s">
         <v>292</v>
       </c>
@@ -18600,6 +18861,9 @@
       </c>
       <c r="S101">
         <v>403</v>
+      </c>
+      <c r="T101">
+        <v>-1</v>
       </c>
       <c r="U101" t="s">
         <v>293</v>
@@ -18821,6 +19085,9 @@
       <c r="S105">
         <v>500</v>
       </c>
+      <c r="T105">
+        <v>-1</v>
+      </c>
       <c r="U105" t="s">
         <v>293</v>
       </c>
@@ -18906,6 +19173,9 @@
       <c r="S106">
         <v>501</v>
       </c>
+      <c r="T106">
+        <v>-1</v>
+      </c>
       <c r="U106" t="s">
         <v>292</v>
       </c>
@@ -18991,6 +19261,9 @@
       <c r="S107">
         <v>502</v>
       </c>
+      <c r="T107">
+        <v>-1</v>
+      </c>
       <c r="U107" t="s">
         <v>292</v>
       </c>
@@ -19076,6 +19349,9 @@
       <c r="S108">
         <v>503</v>
       </c>
+      <c r="T108">
+        <v>-1</v>
+      </c>
       <c r="U108" t="s">
         <v>292</v>
       </c>
@@ -19202,6 +19478,9 @@
       <c r="S111">
         <v>600</v>
       </c>
+      <c r="T111">
+        <v>-1</v>
+      </c>
       <c r="U111" t="s">
         <v>292</v>
       </c>
@@ -19286,6 +19565,9 @@
       </c>
       <c r="S112">
         <v>601</v>
+      </c>
+      <c r="T112">
+        <v>-1</v>
       </c>
       <c r="U112" t="s">
         <v>293</v>

</xml_diff>

<commit_message>
more updates from Eoghan
</commit_message>
<xml_diff>
--- a/lighterFluid/inputs/lnlArrayMasterSheet.xlsx
+++ b/lighterFluid/inputs/lnlArrayMasterSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eoghanoc\source\repos\lighterFluid\lighterFluid\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B01F49-8D93-4379-859C-686FCB62F7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22801731-ACAC-43D6-B9BF-AFFD81F9175B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1620" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-1575" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="templateLookup" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2870" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2910" uniqueCount="308">
   <si>
     <t>Flow</t>
   </si>
@@ -928,6 +928,42 @@
   </si>
   <si>
     <t>VCCSA_HC</t>
+  </si>
+  <si>
+    <t>array_pbist_hry_tito_atom_direct_ssa_list</t>
+  </si>
+  <si>
+    <t>array_pbist_hry_tito_atom_direct_lsa_list</t>
+  </si>
+  <si>
+    <t>array_pbist_hry_tito_atom_indirect_lsa_repairable_list</t>
+  </si>
+  <si>
+    <t>array_pbist_pstrep_atom_sino_direct_lsa_list</t>
+  </si>
+  <si>
+    <t>array_pbist_pstrep_atom_sino_direct_ssa_list</t>
+  </si>
+  <si>
+    <t>array_pbist_raster_tito_atom_direct_lsa_l2_lru_list</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>array_pbist_raster_tito_atom_direct_ssa_l2_c6s_list</t>
+  </si>
+  <si>
+    <t>array_pbist_raster_tito_atom_direct_ssa_l2_data_list</t>
+  </si>
+  <si>
+    <t>array_pbist_raster_tito_atom_direct_ssa_l2_tsp_list</t>
+  </si>
+  <si>
+    <t>array_pbist_raster_tito_atom_indirect_lsa_list</t>
+  </si>
+  <si>
+    <t>array_pbist_pstrep_atom_sino_indirect_lsa_list</t>
   </si>
 </sst>
 </file>
@@ -2133,8 +2169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F8E28AB-C6A9-4AC0-A975-B939A492DE78}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2611,10 +2647,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AJ101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="T78" sqref="T78"/>
+      <selection pane="bottomLeft" activeCell="AB55" sqref="AB55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2622,13 +2658,14 @@
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="83.5703125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="83.5703125" customWidth="1"/>
     <col min="13" max="13" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="14.7109375" customWidth="1"/>
     <col min="24" max="24" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="71.42578125" bestFit="1" customWidth="1"/>
     <col min="31" max="32" width="71.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2871,6 +2908,9 @@
       <c r="T5">
         <v>1</v>
       </c>
+      <c r="U5" t="s">
+        <v>294</v>
+      </c>
       <c r="X5" t="b">
         <v>0</v>
       </c>
@@ -2882,7 +2922,7 @@
         <v>39</v>
       </c>
       <c r="AA5" t="str">
-        <f t="shared" ref="AA5:AA20" si="1">D6</f>
+        <f t="shared" ref="AA5:AA35" si="1">D6</f>
         <v>SSA_CCF_RASTER_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO0_LLC_DAT_RASTER</v>
       </c>
       <c r="AB5" t="str">
@@ -2902,7 +2942,7 @@
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO0_LLC_TAG_BISR</v>
       </c>
       <c r="AF5" t="str">
-        <f t="shared" ref="AF5:AF20" si="2">D6</f>
+        <f t="shared" ref="AF5:AF35" si="2">D6</f>
         <v>SSA_CCF_RASTER_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO0_LLC_DAT_RASTER</v>
       </c>
       <c r="AG5" t="str">
@@ -2982,6 +3022,9 @@
       <c r="T6">
         <v>1</v>
       </c>
+      <c r="U6" t="s">
+        <v>294</v>
+      </c>
       <c r="X6" t="b">
         <v>0</v>
       </c>
@@ -3081,6 +3124,9 @@
       <c r="T7">
         <v>1</v>
       </c>
+      <c r="U7" t="s">
+        <v>294</v>
+      </c>
       <c r="X7" t="b">
         <v>0</v>
       </c>
@@ -3192,6 +3238,9 @@
       <c r="T8">
         <v>1</v>
       </c>
+      <c r="U8" t="s">
+        <v>294</v>
+      </c>
       <c r="X8" t="b">
         <v>0</v>
       </c>
@@ -3291,6 +3340,9 @@
       <c r="T9">
         <v>1</v>
       </c>
+      <c r="U9" t="s">
+        <v>295</v>
+      </c>
       <c r="X9" t="b">
         <v>0</v>
       </c>
@@ -3402,6 +3454,9 @@
       <c r="T10">
         <v>1</v>
       </c>
+      <c r="U10" t="s">
+        <v>295</v>
+      </c>
       <c r="X10" t="b">
         <v>0</v>
       </c>
@@ -3501,6 +3556,9 @@
       <c r="T11">
         <v>1</v>
       </c>
+      <c r="U11" t="s">
+        <v>294</v>
+      </c>
       <c r="X11" t="b">
         <v>0</v>
       </c>
@@ -3612,6 +3670,9 @@
       <c r="T12">
         <v>1</v>
       </c>
+      <c r="U12" t="s">
+        <v>294</v>
+      </c>
       <c r="X12" t="b">
         <v>0</v>
       </c>
@@ -3711,6 +3772,9 @@
       <c r="T13">
         <v>1</v>
       </c>
+      <c r="U13" t="s">
+        <v>294</v>
+      </c>
       <c r="X13" t="b">
         <v>0</v>
       </c>
@@ -3822,6 +3886,9 @@
       <c r="T14">
         <v>1</v>
       </c>
+      <c r="U14" t="s">
+        <v>294</v>
+      </c>
       <c r="X14" t="b">
         <v>0</v>
       </c>
@@ -3921,6 +3988,9 @@
       <c r="T15">
         <v>1</v>
       </c>
+      <c r="U15" t="s">
+        <v>294</v>
+      </c>
       <c r="X15" t="b">
         <v>0</v>
       </c>
@@ -4032,6 +4102,9 @@
       <c r="T16">
         <v>1</v>
       </c>
+      <c r="U16" t="s">
+        <v>294</v>
+      </c>
       <c r="X16" t="b">
         <v>0</v>
       </c>
@@ -4131,6 +4204,9 @@
       <c r="T17">
         <v>1</v>
       </c>
+      <c r="U17" t="s">
+        <v>295</v>
+      </c>
       <c r="X17" t="b">
         <v>0</v>
       </c>
@@ -4242,6 +4318,9 @@
       <c r="T18">
         <v>1</v>
       </c>
+      <c r="U18" t="s">
+        <v>295</v>
+      </c>
       <c r="X18" t="b">
         <v>0</v>
       </c>
@@ -4341,6 +4420,9 @@
       <c r="T19">
         <v>1</v>
       </c>
+      <c r="U19" t="s">
+        <v>294</v>
+      </c>
       <c r="X19" t="b">
         <v>0</v>
       </c>
@@ -4452,6 +4534,9 @@
       <c r="T20">
         <v>1</v>
       </c>
+      <c r="U20" t="s">
+        <v>294</v>
+      </c>
       <c r="X20" t="b">
         <v>0</v>
       </c>
@@ -4551,6 +4636,9 @@
       <c r="T21">
         <v>1</v>
       </c>
+      <c r="U21" t="s">
+        <v>294</v>
+      </c>
       <c r="X21" t="b">
         <v>0</v>
       </c>
@@ -4562,7 +4650,7 @@
         <v>39</v>
       </c>
       <c r="AA21" t="str">
-        <f t="shared" ref="AA21:AA35" si="8">D22</f>
+        <f t="shared" si="1"/>
         <v>SSA_CCF_RASTER_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO2_LLC_DAT_RASTER</v>
       </c>
       <c r="AB21" t="str">
@@ -4582,7 +4670,7 @@
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO2_LLC_TAG_BISR</v>
       </c>
       <c r="AF21" t="str">
-        <f t="shared" ref="AF21:AF35" si="9">D22</f>
+        <f t="shared" si="2"/>
         <v>SSA_CCF_RASTER_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO2_LLC_DAT_RASTER</v>
       </c>
       <c r="AG21" t="str">
@@ -4662,18 +4750,21 @@
       <c r="T22">
         <v>1</v>
       </c>
+      <c r="U22" t="s">
+        <v>294</v>
+      </c>
       <c r="X22" t="b">
         <v>0</v>
       </c>
       <c r="Y22">
-        <f t="shared" ref="Y22:Y36" si="10">COUNTA(AA22:AJ22)</f>
+        <f t="shared" ref="Y22:Y36" si="8">COUNTA(AA22:AJ22)</f>
         <v>6</v>
       </c>
       <c r="Z22">
         <v>1</v>
       </c>
       <c r="AA22" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO2_LLC_TAG_BISR</v>
       </c>
       <c r="AB22" t="str">
@@ -4693,7 +4784,7 @@
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO2_LLC_TAG_BISR</v>
       </c>
       <c r="AF22" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO2_LLC_TAG_BISR</v>
       </c>
     </row>
@@ -4761,18 +4852,21 @@
       <c r="T23">
         <v>1</v>
       </c>
+      <c r="U23" t="s">
+        <v>294</v>
+      </c>
       <c r="X23" t="b">
         <v>0</v>
       </c>
       <c r="Y23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="Z23" t="s">
         <v>39</v>
       </c>
       <c r="AA23" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>SSA_CCF_RASTER_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO2_LLC_TAG_RASTER</v>
       </c>
       <c r="AB23" t="str">
@@ -4792,7 +4886,7 @@
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO2_SAR_BISR</v>
       </c>
       <c r="AF23" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>SSA_CCF_RASTER_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO2_LLC_TAG_RASTER</v>
       </c>
       <c r="AG23" t="str">
@@ -4872,18 +4966,21 @@
       <c r="T24">
         <v>1</v>
       </c>
+      <c r="U24" t="s">
+        <v>294</v>
+      </c>
       <c r="X24" t="b">
         <v>0</v>
       </c>
       <c r="Y24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="Z24">
         <v>1</v>
       </c>
       <c r="AA24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO2_SAR_BISR</v>
       </c>
       <c r="AB24" t="str">
@@ -4903,7 +5000,7 @@
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO2_SAR_BISR</v>
       </c>
       <c r="AF24" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO2_SAR_BISR</v>
       </c>
     </row>
@@ -4971,18 +5068,21 @@
       <c r="T25">
         <v>1</v>
       </c>
+      <c r="U25" t="s">
+        <v>295</v>
+      </c>
       <c r="X25" t="b">
         <v>0</v>
       </c>
       <c r="Y25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="Z25" t="s">
         <v>39</v>
       </c>
       <c r="AA25" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>SSA_CCF_RASTER_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO2_SAR_RASTER</v>
       </c>
       <c r="AB25" t="str">
@@ -5002,7 +5102,7 @@
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_NOM_LFM_CBO2_LSA_ALL</v>
       </c>
       <c r="AF25" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>SSA_CCF_RASTER_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO2_SAR_RASTER</v>
       </c>
       <c r="AG25" t="str">
@@ -5082,18 +5182,21 @@
       <c r="T26">
         <v>1</v>
       </c>
+      <c r="U26" t="s">
+        <v>295</v>
+      </c>
       <c r="X26" t="b">
         <v>0</v>
       </c>
       <c r="Y26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="Z26">
         <v>1</v>
       </c>
       <c r="AA26" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_NOM_LFM_CBO2_LSA_ALL</v>
       </c>
       <c r="AB26" t="str">
@@ -5113,7 +5216,7 @@
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_NOM_LFM_CBO2_LSA_ALL</v>
       </c>
       <c r="AF26" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_NOM_LFM_CBO2_LSA_ALL</v>
       </c>
     </row>
@@ -5181,18 +5284,21 @@
       <c r="T27">
         <v>1</v>
       </c>
+      <c r="U27" t="s">
+        <v>294</v>
+      </c>
       <c r="X27" t="b">
         <v>0</v>
       </c>
       <c r="Y27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="Z27" t="s">
         <v>39</v>
       </c>
       <c r="AA27" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>LSA_CCF_RASTER_E_BEGIN_TITO_CLR_NOM_LFM_CBO2_LSA_ALL</v>
       </c>
       <c r="AB27" t="str">
@@ -5212,7 +5318,7 @@
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO3_LLC_DAT_BISR</v>
       </c>
       <c r="AF27" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>LSA_CCF_RASTER_E_BEGIN_TITO_CLR_NOM_LFM_CBO2_LSA_ALL</v>
       </c>
       <c r="AG27" t="str">
@@ -5292,18 +5398,21 @@
       <c r="T28">
         <v>1</v>
       </c>
+      <c r="U28" t="s">
+        <v>294</v>
+      </c>
       <c r="X28" t="b">
         <v>0</v>
       </c>
       <c r="Y28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="Z28">
         <v>1</v>
       </c>
       <c r="AA28" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO3_LLC_DAT_BISR</v>
       </c>
       <c r="AB28" t="str">
@@ -5323,7 +5432,7 @@
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO3_LLC_DAT_BISR</v>
       </c>
       <c r="AF28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO3_LLC_DAT_BISR</v>
       </c>
     </row>
@@ -5391,18 +5500,21 @@
       <c r="T29">
         <v>1</v>
       </c>
+      <c r="U29" t="s">
+        <v>294</v>
+      </c>
       <c r="X29" t="b">
         <v>0</v>
       </c>
       <c r="Y29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="Z29" t="s">
         <v>39</v>
       </c>
       <c r="AA29" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>SSA_CCF_RASTER_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO3_LLC_DAT_RASTER</v>
       </c>
       <c r="AB29" t="str">
@@ -5422,7 +5534,7 @@
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO3_LLC_TAG_BISR</v>
       </c>
       <c r="AF29" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>SSA_CCF_RASTER_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO3_LLC_DAT_RASTER</v>
       </c>
       <c r="AG29" t="str">
@@ -5502,18 +5614,21 @@
       <c r="T30">
         <v>1</v>
       </c>
+      <c r="U30" t="s">
+        <v>294</v>
+      </c>
       <c r="X30" t="b">
         <v>0</v>
       </c>
       <c r="Y30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="Z30">
         <v>1</v>
       </c>
       <c r="AA30" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO3_LLC_TAG_BISR</v>
       </c>
       <c r="AB30" t="str">
@@ -5533,7 +5648,7 @@
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO3_LLC_TAG_BISR</v>
       </c>
       <c r="AF30" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO3_LLC_TAG_BISR</v>
       </c>
     </row>
@@ -5601,18 +5716,21 @@
       <c r="T31">
         <v>1</v>
       </c>
+      <c r="U31" t="s">
+        <v>294</v>
+      </c>
       <c r="X31" t="b">
         <v>0</v>
       </c>
       <c r="Y31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="Z31" t="s">
         <v>39</v>
       </c>
       <c r="AA31" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>SSA_CCF_RASTER_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO3_LLC_TAG_RASTER</v>
       </c>
       <c r="AB31" t="str">
@@ -5632,7 +5750,7 @@
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO3_SAR_BISR</v>
       </c>
       <c r="AF31" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>SSA_CCF_RASTER_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO3_LLC_TAG_RASTER</v>
       </c>
       <c r="AG31" t="str">
@@ -5712,18 +5830,21 @@
       <c r="T32">
         <v>1</v>
       </c>
+      <c r="U32" t="s">
+        <v>294</v>
+      </c>
       <c r="X32" t="b">
         <v>0</v>
       </c>
       <c r="Y32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="Z32">
         <v>1</v>
       </c>
       <c r="AA32" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO3_SAR_BISR</v>
       </c>
       <c r="AB32" t="str">
@@ -5743,7 +5864,7 @@
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO3_SAR_BISR</v>
       </c>
       <c r="AF32" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO3_SAR_BISR</v>
       </c>
     </row>
@@ -5811,18 +5932,21 @@
       <c r="T33">
         <v>1</v>
       </c>
+      <c r="U33" t="s">
+        <v>295</v>
+      </c>
       <c r="X33" t="b">
         <v>0</v>
       </c>
       <c r="Y33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="Z33" t="s">
         <v>39</v>
       </c>
       <c r="AA33" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>SSA_CCF_RASTER_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO3_SAR_RASTER</v>
       </c>
       <c r="AB33" t="str">
@@ -5842,7 +5966,7 @@
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_NOM_LFM_CBO3_LSA_ALL</v>
       </c>
       <c r="AF33" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>SSA_CCF_RASTER_E_BEGIN_TITO_CLRSS_NOM_LFM_CBO3_SAR_RASTER</v>
       </c>
       <c r="AG33" t="str">
@@ -5922,18 +6046,21 @@
       <c r="T34">
         <v>1</v>
       </c>
+      <c r="U34" t="s">
+        <v>295</v>
+      </c>
       <c r="X34" t="b">
         <v>0</v>
       </c>
       <c r="Y34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="Z34">
         <v>1</v>
       </c>
       <c r="AA34" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_NOM_LFM_CBO3_LSA_ALL</v>
       </c>
       <c r="AB34" t="str">
@@ -5953,7 +6080,7 @@
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_NOM_LFM_CBO3_LSA_ALL</v>
       </c>
       <c r="AF34" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_NOM_LFM_CBO3_LSA_ALL</v>
       </c>
     </row>
@@ -6021,18 +6148,21 @@
       <c r="T35">
         <v>1</v>
       </c>
+      <c r="U35" t="s">
+        <v>294</v>
+      </c>
       <c r="X35" t="b">
         <v>0</v>
       </c>
       <c r="Y35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="Z35" t="s">
         <v>39</v>
       </c>
       <c r="AA35" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>LSA_CCF_RASTER_E_BEGIN_TITO_CLR_NOM_LFM_CBO3_LSA_ALL</v>
       </c>
       <c r="AB35">
@@ -6048,7 +6178,7 @@
         <v>1</v>
       </c>
       <c r="AF35" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>LSA_CCF_RASTER_E_BEGIN_TITO_CLR_NOM_LFM_CBO3_LSA_ALL</v>
       </c>
       <c r="AG35" t="str">
@@ -6128,11 +6258,14 @@
       <c r="T36">
         <v>1</v>
       </c>
+      <c r="U36" t="s">
+        <v>294</v>
+      </c>
       <c r="X36" t="b">
         <v>0</v>
       </c>
       <c r="Y36">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="Z36">
@@ -6279,15 +6412,15 @@
         <v>120</v>
       </c>
       <c r="AA39" t="str">
-        <f>D40</f>
+        <f t="shared" ref="AA39:AA53" si="9">D40</f>
         <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO0_LLC_TAG</v>
       </c>
       <c r="AB39" t="str">
-        <f>D40</f>
+        <f t="shared" ref="AB39:AB53" si="10">D40</f>
         <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO0_LLC_TAG</v>
       </c>
       <c r="AC39" t="str">
-        <f>D40</f>
+        <f t="shared" ref="AC39:AC53" si="11">D40</f>
         <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO0_LLC_TAG</v>
       </c>
     </row>
@@ -6368,15 +6501,15 @@
         <v>120</v>
       </c>
       <c r="AA40" t="str">
-        <f t="shared" ref="AA40:AA53" si="11">D41</f>
+        <f t="shared" si="9"/>
         <v>LSA_CCF_VFDM_E_BEGIN_X_CLR_X_X_CBO0_RF</v>
       </c>
       <c r="AB40" t="str">
-        <f t="shared" ref="AB40:AB53" si="12">D41</f>
+        <f t="shared" si="10"/>
         <v>LSA_CCF_VFDM_E_BEGIN_X_CLR_X_X_CBO0_RF</v>
       </c>
       <c r="AC40" t="str">
-        <f t="shared" ref="AC40:AC53" si="13">D41</f>
+        <f t="shared" si="11"/>
         <v>LSA_CCF_VFDM_E_BEGIN_X_CLR_X_X_CBO0_RF</v>
       </c>
     </row>
@@ -6457,15 +6590,15 @@
         <v>120</v>
       </c>
       <c r="AA41" t="str">
+        <f t="shared" si="9"/>
+        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO1_LLC_DAT</v>
+      </c>
+      <c r="AB41" t="str">
+        <f t="shared" si="10"/>
+        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO1_LLC_DAT</v>
+      </c>
+      <c r="AC41" t="str">
         <f t="shared" si="11"/>
-        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO1_LLC_DAT</v>
-      </c>
-      <c r="AB41" t="str">
-        <f t="shared" si="12"/>
-        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO1_LLC_DAT</v>
-      </c>
-      <c r="AC41" t="str">
-        <f t="shared" si="13"/>
         <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO1_LLC_DAT</v>
       </c>
     </row>
@@ -6481,7 +6614,7 @@
         <v>iCVFDMTest</v>
       </c>
       <c r="D42" t="str">
-        <f t="shared" ref="D42:D53" si="14">E42&amp;"_"&amp;F42&amp;"_"&amp;G42&amp;"_"&amp;H42&amp;"_"&amp;A42&amp;"_"&amp;I42&amp;"_"&amp;J42&amp;"_"&amp;K42&amp;"_"&amp;L42&amp;"_"&amp;M42</f>
+        <f t="shared" ref="D42:D53" si="12">E42&amp;"_"&amp;F42&amp;"_"&amp;G42&amp;"_"&amp;H42&amp;"_"&amp;A42&amp;"_"&amp;I42&amp;"_"&amp;J42&amp;"_"&amp;K42&amp;"_"&amp;L42&amp;"_"&amp;M42</f>
         <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO1_LLC_DAT</v>
       </c>
       <c r="E42" t="s">
@@ -6546,15 +6679,15 @@
         <v>120</v>
       </c>
       <c r="AA42" t="str">
+        <f t="shared" si="9"/>
+        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO1_LLC_TAG</v>
+      </c>
+      <c r="AB42" t="str">
+        <f t="shared" si="10"/>
+        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO1_LLC_TAG</v>
+      </c>
+      <c r="AC42" t="str">
         <f t="shared" si="11"/>
-        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO1_LLC_TAG</v>
-      </c>
-      <c r="AB42" t="str">
-        <f t="shared" si="12"/>
-        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO1_LLC_TAG</v>
-      </c>
-      <c r="AC42" t="str">
-        <f t="shared" si="13"/>
         <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO1_LLC_TAG</v>
       </c>
     </row>
@@ -6570,7 +6703,7 @@
         <v>iCVFDMTest</v>
       </c>
       <c r="D43" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO1_LLC_TAG</v>
       </c>
       <c r="E43" t="s">
@@ -6635,15 +6768,15 @@
         <v>120</v>
       </c>
       <c r="AA43" t="str">
+        <f t="shared" si="9"/>
+        <v>LSA_CCF_VFDM_E_BEGIN_X_CLR_X_X_CBO1_RF</v>
+      </c>
+      <c r="AB43" t="str">
+        <f t="shared" si="10"/>
+        <v>LSA_CCF_VFDM_E_BEGIN_X_CLR_X_X_CBO1_RF</v>
+      </c>
+      <c r="AC43" t="str">
         <f t="shared" si="11"/>
-        <v>LSA_CCF_VFDM_E_BEGIN_X_CLR_X_X_CBO1_RF</v>
-      </c>
-      <c r="AB43" t="str">
-        <f t="shared" si="12"/>
-        <v>LSA_CCF_VFDM_E_BEGIN_X_CLR_X_X_CBO1_RF</v>
-      </c>
-      <c r="AC43" t="str">
-        <f t="shared" si="13"/>
         <v>LSA_CCF_VFDM_E_BEGIN_X_CLR_X_X_CBO1_RF</v>
       </c>
     </row>
@@ -6659,7 +6792,7 @@
         <v>iCVFDMTest</v>
       </c>
       <c r="D44" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>LSA_CCF_VFDM_E_BEGIN_X_CLR_X_X_CBO1_RF</v>
       </c>
       <c r="E44" t="s">
@@ -6724,15 +6857,15 @@
         <v>120</v>
       </c>
       <c r="AA44" t="str">
+        <f t="shared" si="9"/>
+        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO01_SAR</v>
+      </c>
+      <c r="AB44" t="str">
+        <f t="shared" si="10"/>
+        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO01_SAR</v>
+      </c>
+      <c r="AC44" t="str">
         <f t="shared" si="11"/>
-        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO01_SAR</v>
-      </c>
-      <c r="AB44" t="str">
-        <f t="shared" si="12"/>
-        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO01_SAR</v>
-      </c>
-      <c r="AC44" t="str">
-        <f t="shared" si="13"/>
         <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO01_SAR</v>
       </c>
     </row>
@@ -6748,7 +6881,7 @@
         <v>iCVFDMTest</v>
       </c>
       <c r="D45" t="str">
-        <f t="shared" ref="D45" si="15">E45&amp;"_"&amp;F45&amp;"_"&amp;G45&amp;"_"&amp;H45&amp;"_"&amp;A45&amp;"_"&amp;I45&amp;"_"&amp;J45&amp;"_"&amp;K45&amp;"_"&amp;L45&amp;"_"&amp;M45</f>
+        <f t="shared" ref="D45" si="13">E45&amp;"_"&amp;F45&amp;"_"&amp;G45&amp;"_"&amp;H45&amp;"_"&amp;A45&amp;"_"&amp;I45&amp;"_"&amp;J45&amp;"_"&amp;K45&amp;"_"&amp;L45&amp;"_"&amp;M45</f>
         <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO01_SAR</v>
       </c>
       <c r="E45" t="s">
@@ -6813,15 +6946,15 @@
         <v>120</v>
       </c>
       <c r="AA45" t="str">
+        <f t="shared" si="9"/>
+        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO2_LLC_DAT</v>
+      </c>
+      <c r="AB45" t="str">
+        <f t="shared" si="10"/>
+        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO2_LLC_DAT</v>
+      </c>
+      <c r="AC45" t="str">
         <f t="shared" si="11"/>
-        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO2_LLC_DAT</v>
-      </c>
-      <c r="AB45" t="str">
-        <f t="shared" si="12"/>
-        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO2_LLC_DAT</v>
-      </c>
-      <c r="AC45" t="str">
-        <f t="shared" si="13"/>
         <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO2_LLC_DAT</v>
       </c>
     </row>
@@ -6902,15 +7035,15 @@
         <v>120</v>
       </c>
       <c r="AA46" t="str">
+        <f t="shared" si="9"/>
+        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO2_LLC_TAG</v>
+      </c>
+      <c r="AB46" t="str">
+        <f t="shared" si="10"/>
+        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO2_LLC_TAG</v>
+      </c>
+      <c r="AC46" t="str">
         <f t="shared" si="11"/>
-        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO2_LLC_TAG</v>
-      </c>
-      <c r="AB46" t="str">
-        <f t="shared" si="12"/>
-        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO2_LLC_TAG</v>
-      </c>
-      <c r="AC46" t="str">
-        <f t="shared" si="13"/>
         <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO2_LLC_TAG</v>
       </c>
     </row>
@@ -6991,15 +7124,15 @@
         <v>120</v>
       </c>
       <c r="AA47" t="str">
+        <f t="shared" si="9"/>
+        <v>LSA_CCF_VFDM_E_BEGIN_X_CLR_X_X_CBO2_RF</v>
+      </c>
+      <c r="AB47" t="str">
+        <f t="shared" si="10"/>
+        <v>LSA_CCF_VFDM_E_BEGIN_X_CLR_X_X_CBO2_RF</v>
+      </c>
+      <c r="AC47" t="str">
         <f t="shared" si="11"/>
-        <v>LSA_CCF_VFDM_E_BEGIN_X_CLR_X_X_CBO2_RF</v>
-      </c>
-      <c r="AB47" t="str">
-        <f t="shared" si="12"/>
-        <v>LSA_CCF_VFDM_E_BEGIN_X_CLR_X_X_CBO2_RF</v>
-      </c>
-      <c r="AC47" t="str">
-        <f t="shared" si="13"/>
         <v>LSA_CCF_VFDM_E_BEGIN_X_CLR_X_X_CBO2_RF</v>
       </c>
     </row>
@@ -7080,15 +7213,15 @@
         <v>120</v>
       </c>
       <c r="AA48" t="str">
+        <f t="shared" si="9"/>
+        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO3_LLC_DAT</v>
+      </c>
+      <c r="AB48" t="str">
+        <f t="shared" si="10"/>
+        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO3_LLC_DAT</v>
+      </c>
+      <c r="AC48" t="str">
         <f t="shared" si="11"/>
-        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO3_LLC_DAT</v>
-      </c>
-      <c r="AB48" t="str">
-        <f t="shared" si="12"/>
-        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO3_LLC_DAT</v>
-      </c>
-      <c r="AC48" t="str">
-        <f t="shared" si="13"/>
         <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO3_LLC_DAT</v>
       </c>
     </row>
@@ -7104,7 +7237,7 @@
         <v>iCVFDMTest</v>
       </c>
       <c r="D49" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO3_LLC_DAT</v>
       </c>
       <c r="E49" t="s">
@@ -7169,15 +7302,15 @@
         <v>120</v>
       </c>
       <c r="AA49" t="str">
+        <f t="shared" si="9"/>
+        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO3_LLC_TAG</v>
+      </c>
+      <c r="AB49" t="str">
+        <f t="shared" si="10"/>
+        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO3_LLC_TAG</v>
+      </c>
+      <c r="AC49" t="str">
         <f t="shared" si="11"/>
-        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO3_LLC_TAG</v>
-      </c>
-      <c r="AB49" t="str">
-        <f t="shared" si="12"/>
-        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO3_LLC_TAG</v>
-      </c>
-      <c r="AC49" t="str">
-        <f t="shared" si="13"/>
         <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO3_LLC_TAG</v>
       </c>
     </row>
@@ -7193,7 +7326,7 @@
         <v>iCVFDMTest</v>
       </c>
       <c r="D50" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO3_LLC_TAG</v>
       </c>
       <c r="E50" t="s">
@@ -7258,15 +7391,15 @@
         <v>120</v>
       </c>
       <c r="AA50" t="str">
+        <f t="shared" si="9"/>
+        <v>LSA_CCF_VFDM_E_BEGIN_X_CLR_X_X_CBO3_RF</v>
+      </c>
+      <c r="AB50" t="str">
+        <f t="shared" si="10"/>
+        <v>LSA_CCF_VFDM_E_BEGIN_X_CLR_X_X_CBO3_RF</v>
+      </c>
+      <c r="AC50" t="str">
         <f t="shared" si="11"/>
-        <v>LSA_CCF_VFDM_E_BEGIN_X_CLR_X_X_CBO3_RF</v>
-      </c>
-      <c r="AB50" t="str">
-        <f t="shared" si="12"/>
-        <v>LSA_CCF_VFDM_E_BEGIN_X_CLR_X_X_CBO3_RF</v>
-      </c>
-      <c r="AC50" t="str">
-        <f t="shared" si="13"/>
         <v>LSA_CCF_VFDM_E_BEGIN_X_CLR_X_X_CBO3_RF</v>
       </c>
     </row>
@@ -7282,7 +7415,7 @@
         <v>iCVFDMTest</v>
       </c>
       <c r="D51" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>LSA_CCF_VFDM_E_BEGIN_X_CLR_X_X_CBO3_RF</v>
       </c>
       <c r="E51" t="s">
@@ -7347,15 +7480,15 @@
         <v>120</v>
       </c>
       <c r="AA51" t="str">
+        <f t="shared" si="9"/>
+        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO23_SAR</v>
+      </c>
+      <c r="AB51" t="str">
+        <f t="shared" si="10"/>
+        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO23_SAR</v>
+      </c>
+      <c r="AC51" t="str">
         <f t="shared" si="11"/>
-        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO23_SAR</v>
-      </c>
-      <c r="AB51" t="str">
-        <f t="shared" si="12"/>
-        <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO23_SAR</v>
-      </c>
-      <c r="AC51" t="str">
-        <f t="shared" si="13"/>
         <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO23_SAR</v>
       </c>
     </row>
@@ -7371,7 +7504,7 @@
         <v>iCVFDMTest</v>
       </c>
       <c r="D52" t="str">
-        <f t="shared" ref="D52" si="16">E52&amp;"_"&amp;F52&amp;"_"&amp;G52&amp;"_"&amp;H52&amp;"_"&amp;A52&amp;"_"&amp;I52&amp;"_"&amp;J52&amp;"_"&amp;K52&amp;"_"&amp;L52&amp;"_"&amp;M52</f>
+        <f t="shared" ref="D52" si="14">E52&amp;"_"&amp;F52&amp;"_"&amp;G52&amp;"_"&amp;H52&amp;"_"&amp;A52&amp;"_"&amp;I52&amp;"_"&amp;J52&amp;"_"&amp;K52&amp;"_"&amp;L52&amp;"_"&amp;M52</f>
         <v>SSA_CCF_VFDM_E_BEGIN_X_CLRSS_X_X_CBO23_SAR</v>
       </c>
       <c r="E52" t="s">
@@ -7436,15 +7569,15 @@
         <v>120</v>
       </c>
       <c r="AA52" t="str">
+        <f t="shared" si="9"/>
+        <v>ALL_CCF_UF_E_BEGIN_X_CLRSS_X_X_VFDM_UF</v>
+      </c>
+      <c r="AB52" t="str">
+        <f t="shared" si="10"/>
+        <v>ALL_CCF_UF_E_BEGIN_X_CLRSS_X_X_VFDM_UF</v>
+      </c>
+      <c r="AC52" t="str">
         <f t="shared" si="11"/>
-        <v>ALL_CCF_UF_E_BEGIN_X_CLRSS_X_X_VFDM_UF</v>
-      </c>
-      <c r="AB52" t="str">
-        <f t="shared" si="12"/>
-        <v>ALL_CCF_UF_E_BEGIN_X_CLRSS_X_X_VFDM_UF</v>
-      </c>
-      <c r="AC52" t="str">
-        <f t="shared" si="13"/>
         <v>ALL_CCF_UF_E_BEGIN_X_CLRSS_X_X_VFDM_UF</v>
       </c>
     </row>
@@ -7460,7 +7593,7 @@
         <v>iCUserFuncTest</v>
       </c>
       <c r="D53" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>ALL_CCF_UF_E_BEGIN_X_CLRSS_X_X_VFDM_UF</v>
       </c>
       <c r="E53" t="s">
@@ -7522,15 +7655,15 @@
         <v>120</v>
       </c>
       <c r="AA53" t="str">
+        <f t="shared" si="9"/>
+        <v>ALL_CCF_PATMOD_E_BEGIN_TITO_X_MAX_LFM_REPAIR</v>
+      </c>
+      <c r="AB53" t="str">
+        <f t="shared" si="10"/>
+        <v>ALL_CCF_PATMOD_E_BEGIN_TITO_X_MAX_LFM_REPAIR</v>
+      </c>
+      <c r="AC53" t="str">
         <f t="shared" si="11"/>
-        <v>ALL_CCF_PATMOD_E_BEGIN_TITO_X_MAX_LFM_REPAIR</v>
-      </c>
-      <c r="AB53" t="str">
-        <f t="shared" si="12"/>
-        <v>ALL_CCF_PATMOD_E_BEGIN_TITO_X_MAX_LFM_REPAIR</v>
-      </c>
-      <c r="AC53" t="str">
-        <f t="shared" si="13"/>
         <v>ALL_CCF_PATMOD_E_BEGIN_TITO_X_MAX_LFM_REPAIR</v>
       </c>
     </row>
@@ -7670,7 +7803,7 @@
         <v>PrimeMbistVminSearchTestMethod</v>
       </c>
       <c r="D57" t="str">
-        <f t="shared" ref="D57:D64" si="17">E57&amp;"_"&amp;F57&amp;"_"&amp;G57&amp;"_"&amp;H57&amp;"_"&amp;A57&amp;"_"&amp;I57&amp;"_"&amp;J57&amp;"_"&amp;K57&amp;"_"&amp;L57&amp;"_"&amp;M57</f>
+        <f t="shared" ref="D57:D64" si="15">E57&amp;"_"&amp;F57&amp;"_"&amp;G57&amp;"_"&amp;H57&amp;"_"&amp;A57&amp;"_"&amp;I57&amp;"_"&amp;J57&amp;"_"&amp;K57&amp;"_"&amp;L57&amp;"_"&amp;M57</f>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_LLC_DAT_POST_REPAIR</v>
       </c>
       <c r="E57" t="s">
@@ -7722,6 +7855,9 @@
       <c r="T57">
         <v>1</v>
       </c>
+      <c r="U57" t="s">
+        <v>294</v>
+      </c>
       <c r="X57" t="b">
         <v>0</v>
       </c>
@@ -7733,39 +7869,39 @@
         <v>1</v>
       </c>
       <c r="AA57" t="str">
-        <f t="shared" ref="AA57:AA63" si="18">D58</f>
+        <f t="shared" ref="AA57:AA63" si="16">D58</f>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_LLC_TAG_POST_REPAIR</v>
       </c>
       <c r="AB57" t="str">
-        <f t="shared" ref="AB57:AB63" si="19">D58</f>
+        <f t="shared" ref="AB57:AB63" si="17">D58</f>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_LLC_TAG_POST_REPAIR</v>
       </c>
       <c r="AC57" t="str">
-        <f t="shared" ref="AC57:AC63" si="20">D58</f>
+        <f t="shared" ref="AC57:AC63" si="18">D58</f>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_LLC_TAG_POST_REPAIR</v>
       </c>
       <c r="AD57" t="str">
-        <f t="shared" ref="AD57:AD63" si="21">D58</f>
+        <f t="shared" ref="AD57:AD63" si="19">D58</f>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_LLC_TAG_POST_REPAIR</v>
       </c>
       <c r="AE57" t="str">
-        <f t="shared" ref="AE57:AE63" si="22">D58</f>
+        <f t="shared" ref="AE57:AE63" si="20">D58</f>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_LLC_TAG_POST_REPAIR</v>
       </c>
       <c r="AF57" t="str">
-        <f t="shared" ref="AF57:AF63" si="23">D58</f>
+        <f t="shared" ref="AF57:AF63" si="21">D58</f>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_LLC_TAG_POST_REPAIR</v>
       </c>
       <c r="AG57" t="str">
-        <f t="shared" ref="AG57:AG63" si="24">D58</f>
+        <f t="shared" ref="AG57:AG63" si="22">D58</f>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_LLC_TAG_POST_REPAIR</v>
       </c>
       <c r="AH57" t="str">
-        <f t="shared" ref="AH57:AH63" si="25">D58</f>
+        <f t="shared" ref="AH57:AH63" si="23">D58</f>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_LLC_TAG_POST_REPAIR</v>
       </c>
       <c r="AI57" t="str">
-        <f t="shared" ref="AI57:AI63" si="26">D58</f>
+        <f t="shared" ref="AI57:AI63" si="24">D58</f>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_LLC_TAG_POST_REPAIR</v>
       </c>
     </row>
@@ -7781,7 +7917,7 @@
         <v>PrimeMbistVminSearchTestMethod</v>
       </c>
       <c r="D58" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_LLC_TAG_POST_REPAIR</v>
       </c>
       <c r="E58" t="s">
@@ -7833,50 +7969,53 @@
       <c r="T58">
         <v>1</v>
       </c>
+      <c r="U58" t="s">
+        <v>294</v>
+      </c>
       <c r="X58" t="b">
         <v>0</v>
       </c>
       <c r="Y58">
-        <f t="shared" ref="Y58:Y64" si="27">COUNTA(AA58:AJ58)</f>
+        <f t="shared" ref="Y58:Y64" si="25">COUNTA(AA58:AJ58)</f>
         <v>9</v>
       </c>
       <c r="Z58">
         <v>1</v>
       </c>
       <c r="AA58" t="str">
+        <f t="shared" si="16"/>
+        <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_SAR_POST_REPAIR</v>
+      </c>
+      <c r="AB58" t="str">
+        <f t="shared" si="17"/>
+        <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_SAR_POST_REPAIR</v>
+      </c>
+      <c r="AC58" t="str">
         <f t="shared" si="18"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_SAR_POST_REPAIR</v>
       </c>
-      <c r="AB58" t="str">
+      <c r="AD58" t="str">
         <f t="shared" si="19"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_SAR_POST_REPAIR</v>
       </c>
-      <c r="AC58" t="str">
+      <c r="AE58" t="str">
         <f t="shared" si="20"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_SAR_POST_REPAIR</v>
       </c>
-      <c r="AD58" t="str">
+      <c r="AF58" t="str">
         <f t="shared" si="21"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_SAR_POST_REPAIR</v>
       </c>
-      <c r="AE58" t="str">
+      <c r="AG58" t="str">
         <f t="shared" si="22"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_SAR_POST_REPAIR</v>
       </c>
-      <c r="AF58" t="str">
+      <c r="AH58" t="str">
         <f t="shared" si="23"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_SAR_POST_REPAIR</v>
       </c>
-      <c r="AG58" t="str">
+      <c r="AI58" t="str">
         <f t="shared" si="24"/>
-        <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_SAR_POST_REPAIR</v>
-      </c>
-      <c r="AH58" t="str">
-        <f t="shared" si="25"/>
-        <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_SAR_POST_REPAIR</v>
-      </c>
-      <c r="AI58" t="str">
-        <f t="shared" si="26"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_SAR_POST_REPAIR</v>
       </c>
     </row>
@@ -7892,7 +8031,7 @@
         <v>PrimeMbistVminSearchTestMethod</v>
       </c>
       <c r="D59" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO0_SAR_POST_REPAIR</v>
       </c>
       <c r="E59" t="s">
@@ -7944,50 +8083,53 @@
       <c r="T59">
         <v>1</v>
       </c>
+      <c r="U59" t="s">
+        <v>295</v>
+      </c>
       <c r="X59" t="b">
         <v>0</v>
       </c>
       <c r="Y59">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>9</v>
       </c>
       <c r="Z59">
         <v>1</v>
       </c>
       <c r="AA59" t="str">
+        <f t="shared" si="16"/>
+        <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO0_LSA_ALL_POST_REPAIR</v>
+      </c>
+      <c r="AB59" t="str">
+        <f t="shared" si="17"/>
+        <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO0_LSA_ALL_POST_REPAIR</v>
+      </c>
+      <c r="AC59" t="str">
         <f t="shared" si="18"/>
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO0_LSA_ALL_POST_REPAIR</v>
       </c>
-      <c r="AB59" t="str">
+      <c r="AD59" t="str">
         <f t="shared" si="19"/>
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO0_LSA_ALL_POST_REPAIR</v>
       </c>
-      <c r="AC59" t="str">
+      <c r="AE59" t="str">
         <f t="shared" si="20"/>
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO0_LSA_ALL_POST_REPAIR</v>
       </c>
-      <c r="AD59" t="str">
+      <c r="AF59" t="str">
         <f t="shared" si="21"/>
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO0_LSA_ALL_POST_REPAIR</v>
       </c>
-      <c r="AE59" t="str">
+      <c r="AG59" t="str">
         <f t="shared" si="22"/>
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO0_LSA_ALL_POST_REPAIR</v>
       </c>
-      <c r="AF59" t="str">
+      <c r="AH59" t="str">
         <f t="shared" si="23"/>
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO0_LSA_ALL_POST_REPAIR</v>
       </c>
-      <c r="AG59" t="str">
+      <c r="AI59" t="str">
         <f t="shared" si="24"/>
-        <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO0_LSA_ALL_POST_REPAIR</v>
-      </c>
-      <c r="AH59" t="str">
-        <f t="shared" si="25"/>
-        <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO0_LSA_ALL_POST_REPAIR</v>
-      </c>
-      <c r="AI59" t="str">
-        <f t="shared" si="26"/>
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO0_LSA_ALL_POST_REPAIR</v>
       </c>
     </row>
@@ -8003,7 +8145,7 @@
         <v>PrimeMbistVminSearchTestMethod</v>
       </c>
       <c r="D60" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO0_LSA_ALL_POST_REPAIR</v>
       </c>
       <c r="E60" t="s">
@@ -8055,50 +8197,53 @@
       <c r="T60">
         <v>1</v>
       </c>
+      <c r="U60" t="s">
+        <v>294</v>
+      </c>
       <c r="X60" t="b">
         <v>0</v>
       </c>
       <c r="Y60">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>9</v>
       </c>
       <c r="Z60">
         <v>1</v>
       </c>
       <c r="AA60" t="str">
+        <f t="shared" si="16"/>
+        <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_DAT_POST_REPAIR</v>
+      </c>
+      <c r="AB60" t="str">
+        <f t="shared" si="17"/>
+        <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_DAT_POST_REPAIR</v>
+      </c>
+      <c r="AC60" t="str">
         <f t="shared" si="18"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_DAT_POST_REPAIR</v>
       </c>
-      <c r="AB60" t="str">
+      <c r="AD60" t="str">
         <f t="shared" si="19"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_DAT_POST_REPAIR</v>
       </c>
-      <c r="AC60" t="str">
+      <c r="AE60" t="str">
         <f t="shared" si="20"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_DAT_POST_REPAIR</v>
       </c>
-      <c r="AD60" t="str">
+      <c r="AF60" t="str">
         <f t="shared" si="21"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_DAT_POST_REPAIR</v>
       </c>
-      <c r="AE60" t="str">
+      <c r="AG60" t="str">
         <f t="shared" si="22"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_DAT_POST_REPAIR</v>
       </c>
-      <c r="AF60" t="str">
+      <c r="AH60" t="str">
         <f t="shared" si="23"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_DAT_POST_REPAIR</v>
       </c>
-      <c r="AG60" t="str">
+      <c r="AI60" t="str">
         <f t="shared" si="24"/>
-        <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_DAT_POST_REPAIR</v>
-      </c>
-      <c r="AH60" t="str">
-        <f t="shared" si="25"/>
-        <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_DAT_POST_REPAIR</v>
-      </c>
-      <c r="AI60" t="str">
-        <f t="shared" si="26"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_DAT_POST_REPAIR</v>
       </c>
     </row>
@@ -8114,7 +8259,7 @@
         <v>PrimeMbistVminSearchTestMethod</v>
       </c>
       <c r="D61" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_DAT_POST_REPAIR</v>
       </c>
       <c r="E61" t="s">
@@ -8166,50 +8311,53 @@
       <c r="T61">
         <v>1</v>
       </c>
+      <c r="U61" t="s">
+        <v>294</v>
+      </c>
       <c r="X61" t="b">
         <v>0</v>
       </c>
       <c r="Y61">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>9</v>
       </c>
       <c r="Z61">
         <v>1</v>
       </c>
       <c r="AA61" t="str">
+        <f t="shared" si="16"/>
+        <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_TAG_POST_REPAIR</v>
+      </c>
+      <c r="AB61" t="str">
+        <f t="shared" si="17"/>
+        <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_TAG_POST_REPAIR</v>
+      </c>
+      <c r="AC61" t="str">
         <f t="shared" si="18"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_TAG_POST_REPAIR</v>
       </c>
-      <c r="AB61" t="str">
+      <c r="AD61" t="str">
         <f t="shared" si="19"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_TAG_POST_REPAIR</v>
       </c>
-      <c r="AC61" t="str">
+      <c r="AE61" t="str">
         <f t="shared" si="20"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_TAG_POST_REPAIR</v>
       </c>
-      <c r="AD61" t="str">
+      <c r="AF61" t="str">
         <f t="shared" si="21"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_TAG_POST_REPAIR</v>
       </c>
-      <c r="AE61" t="str">
+      <c r="AG61" t="str">
         <f t="shared" si="22"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_TAG_POST_REPAIR</v>
       </c>
-      <c r="AF61" t="str">
+      <c r="AH61" t="str">
         <f t="shared" si="23"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_TAG_POST_REPAIR</v>
       </c>
-      <c r="AG61" t="str">
+      <c r="AI61" t="str">
         <f t="shared" si="24"/>
-        <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_TAG_POST_REPAIR</v>
-      </c>
-      <c r="AH61" t="str">
-        <f t="shared" si="25"/>
-        <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_TAG_POST_REPAIR</v>
-      </c>
-      <c r="AI61" t="str">
-        <f t="shared" si="26"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_TAG_POST_REPAIR</v>
       </c>
     </row>
@@ -8225,7 +8373,7 @@
         <v>PrimeMbistVminSearchTestMethod</v>
       </c>
       <c r="D62" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_LLC_TAG_POST_REPAIR</v>
       </c>
       <c r="E62" t="s">
@@ -8277,50 +8425,53 @@
       <c r="T62">
         <v>1</v>
       </c>
+      <c r="U62" t="s">
+        <v>294</v>
+      </c>
       <c r="X62" t="b">
         <v>0</v>
       </c>
       <c r="Y62">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>9</v>
       </c>
       <c r="Z62">
         <v>1</v>
       </c>
       <c r="AA62" t="str">
+        <f t="shared" si="16"/>
+        <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_SAR_POST_REPAIR</v>
+      </c>
+      <c r="AB62" t="str">
+        <f t="shared" si="17"/>
+        <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_SAR_POST_REPAIR</v>
+      </c>
+      <c r="AC62" t="str">
         <f t="shared" si="18"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_SAR_POST_REPAIR</v>
       </c>
-      <c r="AB62" t="str">
+      <c r="AD62" t="str">
         <f t="shared" si="19"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_SAR_POST_REPAIR</v>
       </c>
-      <c r="AC62" t="str">
+      <c r="AE62" t="str">
         <f t="shared" si="20"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_SAR_POST_REPAIR</v>
       </c>
-      <c r="AD62" t="str">
+      <c r="AF62" t="str">
         <f t="shared" si="21"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_SAR_POST_REPAIR</v>
       </c>
-      <c r="AE62" t="str">
+      <c r="AG62" t="str">
         <f t="shared" si="22"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_SAR_POST_REPAIR</v>
       </c>
-      <c r="AF62" t="str">
+      <c r="AH62" t="str">
         <f t="shared" si="23"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_SAR_POST_REPAIR</v>
       </c>
-      <c r="AG62" t="str">
+      <c r="AI62" t="str">
         <f t="shared" si="24"/>
-        <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_SAR_POST_REPAIR</v>
-      </c>
-      <c r="AH62" t="str">
-        <f t="shared" si="25"/>
-        <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_SAR_POST_REPAIR</v>
-      </c>
-      <c r="AI62" t="str">
-        <f t="shared" si="26"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_SAR_POST_REPAIR</v>
       </c>
     </row>
@@ -8336,7 +8487,7 @@
         <v>PrimeMbistVminSearchTestMethod</v>
       </c>
       <c r="D63" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>SSA_CCF_HRY_E_BEGIN_TITO_CLRSS_MAX_LFM_CBO1_SAR_POST_REPAIR</v>
       </c>
       <c r="E63" t="s">
@@ -8388,50 +8539,53 @@
       <c r="T63">
         <v>1</v>
       </c>
+      <c r="U63" t="s">
+        <v>295</v>
+      </c>
       <c r="X63" t="b">
         <v>0</v>
       </c>
       <c r="Y63">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>9</v>
       </c>
       <c r="Z63">
         <v>1</v>
       </c>
       <c r="AA63" t="str">
+        <f t="shared" si="16"/>
+        <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO1_LSA_ALL_POST_REPAIR</v>
+      </c>
+      <c r="AB63" t="str">
+        <f t="shared" si="17"/>
+        <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO1_LSA_ALL_POST_REPAIR</v>
+      </c>
+      <c r="AC63" t="str">
         <f t="shared" si="18"/>
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO1_LSA_ALL_POST_REPAIR</v>
       </c>
-      <c r="AB63" t="str">
+      <c r="AD63" t="str">
         <f t="shared" si="19"/>
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO1_LSA_ALL_POST_REPAIR</v>
       </c>
-      <c r="AC63" t="str">
+      <c r="AE63" t="str">
         <f t="shared" si="20"/>
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO1_LSA_ALL_POST_REPAIR</v>
       </c>
-      <c r="AD63" t="str">
+      <c r="AF63" t="str">
         <f t="shared" si="21"/>
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO1_LSA_ALL_POST_REPAIR</v>
       </c>
-      <c r="AE63" t="str">
+      <c r="AG63" t="str">
         <f t="shared" si="22"/>
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO1_LSA_ALL_POST_REPAIR</v>
       </c>
-      <c r="AF63" t="str">
+      <c r="AH63" t="str">
         <f t="shared" si="23"/>
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO1_LSA_ALL_POST_REPAIR</v>
       </c>
-      <c r="AG63" t="str">
+      <c r="AI63" t="str">
         <f t="shared" si="24"/>
-        <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO1_LSA_ALL_POST_REPAIR</v>
-      </c>
-      <c r="AH63" t="str">
-        <f t="shared" si="25"/>
-        <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO1_LSA_ALL_POST_REPAIR</v>
-      </c>
-      <c r="AI63" t="str">
-        <f t="shared" si="26"/>
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO1_LSA_ALL_POST_REPAIR</v>
       </c>
     </row>
@@ -8447,7 +8601,7 @@
         <v>PrimeMbistVminSearchTestMethod</v>
       </c>
       <c r="D64" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>LSA_CCF_HRY_E_BEGIN_TITO_CLR_MAX_LFM_CBO1_LSA_ALL_POST_REPAIR</v>
       </c>
       <c r="E64" t="s">
@@ -8499,11 +8653,14 @@
       <c r="T64">
         <v>1</v>
       </c>
+      <c r="U64" t="s">
+        <v>294</v>
+      </c>
       <c r="X64" t="b">
         <v>0</v>
       </c>
       <c r="Y64">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>9</v>
       </c>
       <c r="Z64">
@@ -8591,7 +8748,7 @@
         <v>PrimeVminSearchTestMethod</v>
       </c>
       <c r="D68" t="str">
-        <f t="shared" ref="D68:D73" si="28">E68&amp;"_"&amp;F68&amp;"_"&amp;G68&amp;"_"&amp;H68&amp;"_"&amp;A68&amp;"_"&amp;I68&amp;"_"&amp;J68&amp;"_"&amp;K68&amp;"_"&amp;L68&amp;"_"&amp;M68</f>
+        <f t="shared" ref="D68:D73" si="26">E68&amp;"_"&amp;F68&amp;"_"&amp;G68&amp;"_"&amp;H68&amp;"_"&amp;A68&amp;"_"&amp;I68&amp;"_"&amp;J68&amp;"_"&amp;K68&amp;"_"&amp;L68&amp;"_"&amp;M68</f>
         <v>SSA_CCF_VMIN_K_PREHVQK_TITO_CLRSS_MIN_LFM_CBO</v>
       </c>
       <c r="E68" t="s">
@@ -8653,7 +8810,7 @@
         <v>0</v>
       </c>
       <c r="Y68">
-        <f t="shared" ref="Y68:Y73" si="29">COUNTA(AA68:AJ68)</f>
+        <f t="shared" ref="Y68:Y73" si="27">COUNTA(AA68:AJ68)</f>
         <v>2</v>
       </c>
       <c r="Z68">
@@ -8680,7 +8837,7 @@
         <v>PrimeVminSearchTestMethod</v>
       </c>
       <c r="D69" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>SSA_CCF_VMIN_K_PREHVQK_TITO_CLRSS_MIN_LFM_PMA</v>
       </c>
       <c r="E69" t="s">
@@ -8742,7 +8899,7 @@
         <v>0</v>
       </c>
       <c r="Y69">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>2</v>
       </c>
       <c r="Z69">
@@ -8769,7 +8926,7 @@
         <v>PrimeVminSearchTestMethod</v>
       </c>
       <c r="D70" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>LSA_CCF_VMIN_K_PREHVQK_TITO_CLR_MIN_LFM_CBO</v>
       </c>
       <c r="E70" t="s">
@@ -8831,7 +8988,7 @@
         <v>0</v>
       </c>
       <c r="Y70">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>2</v>
       </c>
       <c r="Z70">
@@ -8858,7 +9015,7 @@
         <v>PrimeVminSearchTestMethod</v>
       </c>
       <c r="D71" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>LSA_CCF_VMIN_K_PREHVQK_TITO_CLR_MIN_LFM_SBO</v>
       </c>
       <c r="E71" t="s">
@@ -8920,7 +9077,7 @@
         <v>0</v>
       </c>
       <c r="Y71">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>2</v>
       </c>
       <c r="Z71">
@@ -8947,7 +9104,7 @@
         <v>PrimeVminSearchTestMethod</v>
       </c>
       <c r="D72" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>ROM_CCF_VMIN_K_PREHVQK_TITO_CLR_MIN_LFM_PMA</v>
       </c>
       <c r="E72" t="s">
@@ -9009,7 +9166,7 @@
         <v>0</v>
       </c>
       <c r="Y72">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>2</v>
       </c>
       <c r="Z72">
@@ -9036,7 +9193,7 @@
         <v>PrimeVminSearchTestMethod</v>
       </c>
       <c r="D73" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>ROM_CCF_VMIN_K_PREHVQK_TITO_CLR_MIN_LFM_SBO</v>
       </c>
       <c r="E73" t="s">
@@ -9098,7 +9255,7 @@
         <v>0</v>
       </c>
       <c r="Y73">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>2</v>
       </c>
       <c r="Z73">
@@ -9212,7 +9369,7 @@
         <v>0</v>
       </c>
       <c r="Y76">
-        <f t="shared" ref="Y76:Y77" si="30">COUNTA(AA76:AJ76)</f>
+        <f t="shared" ref="Y76:Y77" si="28">COUNTA(AA76:AJ76)</f>
         <v>4</v>
       </c>
       <c r="Z76" t="s">
@@ -9306,7 +9463,7 @@
         <v>0</v>
       </c>
       <c r="Y77">
-        <f t="shared" si="30"/>
+        <f t="shared" si="28"/>
         <v>4</v>
       </c>
       <c r="Z77" t="s">
@@ -9367,7 +9524,7 @@
         <v>PrimeVminSearchTestMethod</v>
       </c>
       <c r="D80" t="str">
-        <f t="shared" ref="D80:D85" si="31">E80&amp;"_"&amp;F80&amp;"_"&amp;G80&amp;"_"&amp;H80&amp;"_"&amp;A80&amp;"_"&amp;I80&amp;"_"&amp;J80&amp;"_"&amp;K80&amp;"_"&amp;L80&amp;"_"&amp;M80</f>
+        <f t="shared" ref="D80:D85" si="29">E80&amp;"_"&amp;F80&amp;"_"&amp;G80&amp;"_"&amp;H80&amp;"_"&amp;A80&amp;"_"&amp;I80&amp;"_"&amp;J80&amp;"_"&amp;K80&amp;"_"&amp;L80&amp;"_"&amp;M80</f>
         <v>SSA_CCF_VMIN_K_POSTHVQK_TITO_CLRSS_MIN_LFM_CBO</v>
       </c>
       <c r="E80" t="s">
@@ -9429,7 +9586,7 @@
         <v>0</v>
       </c>
       <c r="Y80">
-        <f t="shared" ref="Y80:Y85" si="32">COUNTA(AA80:AJ80)</f>
+        <f t="shared" ref="Y80:Y85" si="30">COUNTA(AA80:AJ80)</f>
         <v>2</v>
       </c>
       <c r="Z80">
@@ -9456,7 +9613,7 @@
         <v>PrimeVminSearchTestMethod</v>
       </c>
       <c r="D81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="29"/>
         <v>SSA_CCF_VMIN_K_POSTHVQK_TITO_CLRSS_MIN_LFM_PMA</v>
       </c>
       <c r="E81" t="s">
@@ -9518,7 +9675,7 @@
         <v>0</v>
       </c>
       <c r="Y81">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>2</v>
       </c>
       <c r="Z81">
@@ -9545,7 +9702,7 @@
         <v>PrimeVminSearchTestMethod</v>
       </c>
       <c r="D82" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="29"/>
         <v>LSA_CCF_VMIN_K_POSTHVQK_TITO_CLR_MIN_LFM_CBO</v>
       </c>
       <c r="E82" t="s">
@@ -9607,7 +9764,7 @@
         <v>0</v>
       </c>
       <c r="Y82">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>2</v>
       </c>
       <c r="Z82">
@@ -9634,7 +9791,7 @@
         <v>PrimeVminSearchTestMethod</v>
       </c>
       <c r="D83" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="29"/>
         <v>LSA_CCF_VMIN_K_POSTHVQK_TITO_CLR_MIN_LFM_SBO</v>
       </c>
       <c r="E83" t="s">
@@ -9696,7 +9853,7 @@
         <v>0</v>
       </c>
       <c r="Y83">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>2</v>
       </c>
       <c r="Z83">
@@ -9723,7 +9880,7 @@
         <v>PrimeVminSearchTestMethod</v>
       </c>
       <c r="D84" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="29"/>
         <v>ROM_CCF_VMIN_K_POSTHVQK_TITO_CLR_MIN_LFM_PMA</v>
       </c>
       <c r="E84" t="s">
@@ -9785,7 +9942,7 @@
         <v>0</v>
       </c>
       <c r="Y84">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>2</v>
       </c>
       <c r="Z84">
@@ -9812,7 +9969,7 @@
         <v>PrimeVminSearchTestMethod</v>
       </c>
       <c r="D85" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="29"/>
         <v>ROM_CCF_VMIN_K_POSTHVQK_TITO_CLR_MIN_LFM_SBO</v>
       </c>
       <c r="E85" t="s">
@@ -9874,7 +10031,7 @@
         <v>0</v>
       </c>
       <c r="Y85">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>2</v>
       </c>
       <c r="Z85">
@@ -9935,7 +10092,7 @@
         <v>32</v>
       </c>
       <c r="Y88">
-        <f t="shared" ref="Y88" si="33">COUNTA(AA88:AJ88)</f>
+        <f t="shared" ref="Y88" si="31">COUNTA(AA88:AJ88)</f>
         <v>2</v>
       </c>
       <c r="Z88">
@@ -9962,7 +10119,7 @@
         <v>PrimeVminSearchTestMethod</v>
       </c>
       <c r="D89" t="str">
-        <f t="shared" ref="D89:D94" si="34">E89&amp;"_"&amp;F89&amp;"_"&amp;G89&amp;"_"&amp;H89&amp;"_"&amp;A89&amp;"_"&amp;I89&amp;"_"&amp;J89&amp;"_"&amp;K89&amp;"_"&amp;L89&amp;"_"&amp;M89</f>
+        <f t="shared" ref="D89:D94" si="32">E89&amp;"_"&amp;F89&amp;"_"&amp;G89&amp;"_"&amp;H89&amp;"_"&amp;A89&amp;"_"&amp;I89&amp;"_"&amp;J89&amp;"_"&amp;K89&amp;"_"&amp;L89&amp;"_"&amp;M89</f>
         <v>SSA_CCF_VMIN_K_END_TITO_CLRSS_MIN_LFM_CBO</v>
       </c>
       <c r="E89" t="s">
@@ -10024,7 +10181,7 @@
         <v>0</v>
       </c>
       <c r="Y89">
-        <f t="shared" ref="Y89:Y94" si="35">COUNTA(AA89:AJ89)</f>
+        <f t="shared" ref="Y89:Y94" si="33">COUNTA(AA89:AJ89)</f>
         <v>2</v>
       </c>
       <c r="Z89">
@@ -10051,7 +10208,7 @@
         <v>PrimeVminSearchTestMethod</v>
       </c>
       <c r="D90" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>SSA_CCF_VMIN_K_END_TITO_CLRSS_MIN_LFM_PMA</v>
       </c>
       <c r="E90" t="s">
@@ -10113,7 +10270,7 @@
         <v>0</v>
       </c>
       <c r="Y90">
-        <f t="shared" si="35"/>
+        <f t="shared" si="33"/>
         <v>2</v>
       </c>
       <c r="Z90">
@@ -10140,7 +10297,7 @@
         <v>PrimeVminSearchTestMethod</v>
       </c>
       <c r="D91" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>LSA_CCF_VMIN_K_END_TITO_CLR_MIN_LFM_CBO</v>
       </c>
       <c r="E91" t="s">
@@ -10202,7 +10359,7 @@
         <v>0</v>
       </c>
       <c r="Y91">
-        <f t="shared" si="35"/>
+        <f t="shared" si="33"/>
         <v>2</v>
       </c>
       <c r="Z91">
@@ -10229,7 +10386,7 @@
         <v>PrimeVminSearchTestMethod</v>
       </c>
       <c r="D92" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>LSA_CCF_VMIN_K_END_TITO_CLR_MIN_LFM_SBO</v>
       </c>
       <c r="E92" t="s">
@@ -10291,7 +10448,7 @@
         <v>0</v>
       </c>
       <c r="Y92">
-        <f t="shared" si="35"/>
+        <f t="shared" si="33"/>
         <v>2</v>
       </c>
       <c r="Z92">
@@ -10318,7 +10475,7 @@
         <v>PrimeVminSearchTestMethod</v>
       </c>
       <c r="D93" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>ROM_CCF_VMIN_K_END_TITO_CLR_MIN_LFM_PMA</v>
       </c>
       <c r="E93" t="s">
@@ -10380,7 +10537,7 @@
         <v>0</v>
       </c>
       <c r="Y93">
-        <f t="shared" si="35"/>
+        <f t="shared" si="33"/>
         <v>2</v>
       </c>
       <c r="Z93">
@@ -10407,7 +10564,7 @@
         <v>PrimeVminSearchTestMethod</v>
       </c>
       <c r="D94" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>ROM_CCF_VMIN_K_END_TITO_CLR_MIN_LFM_SBO</v>
       </c>
       <c r="E94" t="s">
@@ -10469,7 +10626,7 @@
         <v>0</v>
       </c>
       <c r="Y94">
-        <f t="shared" si="35"/>
+        <f t="shared" si="33"/>
         <v>2</v>
       </c>
       <c r="Z94">
@@ -10512,7 +10669,7 @@
         <v>32</v>
       </c>
       <c r="Y96">
-        <f t="shared" ref="Y96" si="36">COUNTA(AA96:AJ96)</f>
+        <f t="shared" ref="Y96" si="34">COUNTA(AA96:AJ96)</f>
         <v>2</v>
       </c>
       <c r="Z96">
@@ -10598,7 +10755,7 @@
         <v>0</v>
       </c>
       <c r="Y97">
-        <f t="shared" ref="Y97:Y98" si="37">COUNTA(AA97:AJ97)</f>
+        <f t="shared" ref="Y97:Y98" si="35">COUNTA(AA97:AJ97)</f>
         <v>2</v>
       </c>
       <c r="Z97">
@@ -10686,7 +10843,7 @@
         <v>0</v>
       </c>
       <c r="Y98">
-        <f t="shared" si="37"/>
+        <f t="shared" si="35"/>
         <v>2</v>
       </c>
       <c r="Z98">
@@ -10748,8 +10905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E78E7DAD-E2E3-41CA-AC6B-36D49F2F3F66}">
   <dimension ref="A1:AO115"/>
   <sheetViews>
-    <sheetView topLeftCell="E79" workbookViewId="0">
-      <selection activeCell="T96" sqref="T96"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="P76" sqref="P76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10757,13 +10914,18 @@
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.140625" customWidth="1"/>
     <col min="4" max="4" width="73.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="12" width="9.140625" customWidth="1"/>
-    <col min="13" max="13" width="25" bestFit="1" customWidth="1"/>
-    <col min="14" max="20" width="9.140625" customWidth="1"/>
+    <col min="5" max="12" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="25" hidden="1" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" customWidth="1"/>
+    <col min="16" max="16" width="76.28515625" customWidth="1"/>
+    <col min="17" max="19" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" customWidth="1"/>
     <col min="21" max="21" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="28" width="9.140625" customWidth="1"/>
-    <col min="32" max="32" width="25.42578125" customWidth="1"/>
-    <col min="33" max="33" width="28.28515625" customWidth="1"/>
+    <col min="29" max="31" width="0" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="25.42578125" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="28.28515625" hidden="1" customWidth="1"/>
+    <col min="34" max="41" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
@@ -11046,7 +11208,7 @@
         <v>37</v>
       </c>
       <c r="P5" t="s">
-        <v>38</v>
+        <v>296</v>
       </c>
       <c r="Q5">
         <v>60</v>
@@ -11058,7 +11220,7 @@
         <v>0</v>
       </c>
       <c r="T5">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC5" t="b">
         <v>0</v>
@@ -11135,7 +11297,7 @@
         <v>37</v>
       </c>
       <c r="P6" t="s">
-        <v>38</v>
+        <v>304</v>
       </c>
       <c r="Q6">
         <v>60</v>
@@ -11147,7 +11309,7 @@
         <v>1</v>
       </c>
       <c r="T6">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y6" t="s">
         <v>270</v>
@@ -11224,7 +11386,7 @@
         <v>37</v>
       </c>
       <c r="P7" t="s">
-        <v>38</v>
+        <v>304</v>
       </c>
       <c r="Q7">
         <v>60</v>
@@ -11236,7 +11398,7 @@
         <v>2</v>
       </c>
       <c r="T7">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y7" t="s">
         <v>270</v>
@@ -11334,7 +11496,7 @@
         <v>37</v>
       </c>
       <c r="P8" t="s">
-        <v>38</v>
+        <v>304</v>
       </c>
       <c r="Q8">
         <v>60</v>
@@ -11346,7 +11508,7 @@
         <v>3</v>
       </c>
       <c r="T8">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y8" t="s">
         <v>270</v>
@@ -11444,7 +11606,7 @@
         <v>37</v>
       </c>
       <c r="P9" t="s">
-        <v>38</v>
+        <v>303</v>
       </c>
       <c r="Q9">
         <v>60</v>
@@ -11456,7 +11618,7 @@
         <v>4</v>
       </c>
       <c r="T9">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y9" t="s">
         <v>271</v>
@@ -11533,7 +11695,7 @@
         <v>37</v>
       </c>
       <c r="P10" t="s">
-        <v>38</v>
+        <v>303</v>
       </c>
       <c r="Q10">
         <v>60</v>
@@ -11545,7 +11707,7 @@
         <v>5</v>
       </c>
       <c r="T10">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y10" t="s">
         <v>271</v>
@@ -11643,7 +11805,7 @@
         <v>37</v>
       </c>
       <c r="P11" t="s">
-        <v>38</v>
+        <v>303</v>
       </c>
       <c r="Q11">
         <v>60</v>
@@ -11655,7 +11817,7 @@
         <v>6</v>
       </c>
       <c r="T11">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y11" t="s">
         <v>271</v>
@@ -11753,7 +11915,7 @@
         <v>37</v>
       </c>
       <c r="P12" t="s">
-        <v>38</v>
+        <v>305</v>
       </c>
       <c r="Q12">
         <v>60</v>
@@ -11765,7 +11927,7 @@
         <v>7</v>
       </c>
       <c r="T12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y12" t="s">
         <v>272</v>
@@ -11842,7 +12004,7 @@
         <v>37</v>
       </c>
       <c r="P13" t="s">
-        <v>38</v>
+        <v>305</v>
       </c>
       <c r="Q13">
         <v>60</v>
@@ -11854,7 +12016,7 @@
         <v>8</v>
       </c>
       <c r="T13">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y13" t="s">
         <v>272</v>
@@ -11952,7 +12114,7 @@
         <v>37</v>
       </c>
       <c r="P14" t="s">
-        <v>38</v>
+        <v>305</v>
       </c>
       <c r="Q14">
         <v>60</v>
@@ -11964,7 +12126,7 @@
         <v>9</v>
       </c>
       <c r="T14">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y14" t="s">
         <v>272</v>
@@ -12062,7 +12224,7 @@
         <v>37</v>
       </c>
       <c r="P15" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q15">
         <v>60</v>
@@ -12074,7 +12236,7 @@
         <v>10</v>
       </c>
       <c r="T15">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W15" t="s">
         <v>262</v>
@@ -12151,7 +12313,7 @@
         <v>37</v>
       </c>
       <c r="P16" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q16">
         <v>60</v>
@@ -12237,7 +12399,7 @@
         <v>37</v>
       </c>
       <c r="P17" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q17">
         <v>60</v>
@@ -12319,7 +12481,7 @@
         <v>37</v>
       </c>
       <c r="P18" t="s">
-        <v>38</v>
+        <v>300</v>
       </c>
       <c r="Q18">
         <v>60</v>
@@ -12331,7 +12493,7 @@
         <v>13</v>
       </c>
       <c r="T18">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC18" t="b">
         <v>0</v>
@@ -12406,7 +12568,7 @@
         <v>37</v>
       </c>
       <c r="P19" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q19">
         <v>60</v>
@@ -12418,7 +12580,7 @@
         <v>14</v>
       </c>
       <c r="T19">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W19" t="s">
         <v>265</v>
@@ -12541,7 +12703,7 @@
         <v>37</v>
       </c>
       <c r="P22" t="s">
-        <v>38</v>
+        <v>296</v>
       </c>
       <c r="Q22">
         <v>60</v>
@@ -12553,7 +12715,7 @@
         <v>20</v>
       </c>
       <c r="T22">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC22" t="b">
         <v>0</v>
@@ -12630,7 +12792,7 @@
         <v>37</v>
       </c>
       <c r="P23" t="s">
-        <v>38</v>
+        <v>304</v>
       </c>
       <c r="Q23">
         <v>60</v>
@@ -12642,7 +12804,7 @@
         <v>21</v>
       </c>
       <c r="T23">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y23" t="s">
         <v>270</v>
@@ -12719,7 +12881,7 @@
         <v>37</v>
       </c>
       <c r="P24" t="s">
-        <v>38</v>
+        <v>304</v>
       </c>
       <c r="Q24">
         <v>60</v>
@@ -12731,7 +12893,7 @@
         <v>22</v>
       </c>
       <c r="T24">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y24" t="s">
         <v>270</v>
@@ -12829,7 +12991,7 @@
         <v>37</v>
       </c>
       <c r="P25" t="s">
-        <v>38</v>
+        <v>304</v>
       </c>
       <c r="Q25">
         <v>60</v>
@@ -12841,7 +13003,7 @@
         <v>23</v>
       </c>
       <c r="T25">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y25" t="s">
         <v>270</v>
@@ -12939,7 +13101,7 @@
         <v>37</v>
       </c>
       <c r="P26" t="s">
-        <v>38</v>
+        <v>303</v>
       </c>
       <c r="Q26">
         <v>60</v>
@@ -12951,7 +13113,7 @@
         <v>24</v>
       </c>
       <c r="T26">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y26" t="s">
         <v>271</v>
@@ -13028,7 +13190,7 @@
         <v>37</v>
       </c>
       <c r="P27" t="s">
-        <v>38</v>
+        <v>303</v>
       </c>
       <c r="Q27">
         <v>60</v>
@@ -13040,7 +13202,7 @@
         <v>25</v>
       </c>
       <c r="T27">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y27" t="s">
         <v>271</v>
@@ -13138,7 +13300,7 @@
         <v>37</v>
       </c>
       <c r="P28" t="s">
-        <v>38</v>
+        <v>303</v>
       </c>
       <c r="Q28">
         <v>60</v>
@@ -13150,7 +13312,7 @@
         <v>26</v>
       </c>
       <c r="T28">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y28" t="s">
         <v>271</v>
@@ -13248,7 +13410,7 @@
         <v>37</v>
       </c>
       <c r="P29" t="s">
-        <v>38</v>
+        <v>305</v>
       </c>
       <c r="Q29">
         <v>60</v>
@@ -13260,7 +13422,7 @@
         <v>27</v>
       </c>
       <c r="T29">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y29" t="s">
         <v>272</v>
@@ -13337,7 +13499,7 @@
         <v>37</v>
       </c>
       <c r="P30" t="s">
-        <v>38</v>
+        <v>305</v>
       </c>
       <c r="Q30">
         <v>60</v>
@@ -13349,7 +13511,7 @@
         <v>28</v>
       </c>
       <c r="T30">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y30" t="s">
         <v>272</v>
@@ -13447,7 +13609,7 @@
         <v>37</v>
       </c>
       <c r="P31" t="s">
-        <v>38</v>
+        <v>305</v>
       </c>
       <c r="Q31">
         <v>60</v>
@@ -13459,7 +13621,7 @@
         <v>29</v>
       </c>
       <c r="T31">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y31" t="s">
         <v>272</v>
@@ -13557,7 +13719,7 @@
         <v>37</v>
       </c>
       <c r="P32" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q32">
         <v>60</v>
@@ -13569,7 +13731,7 @@
         <v>30</v>
       </c>
       <c r="T32">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W32" t="s">
         <v>262</v>
@@ -13646,7 +13808,7 @@
         <v>37</v>
       </c>
       <c r="P33" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q33">
         <v>60</v>
@@ -13732,7 +13894,7 @@
         <v>37</v>
       </c>
       <c r="P34" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q34">
         <v>60</v>
@@ -13814,7 +13976,7 @@
         <v>37</v>
       </c>
       <c r="P35" t="s">
-        <v>38</v>
+        <v>300</v>
       </c>
       <c r="Q35">
         <v>60</v>
@@ -13826,7 +13988,7 @@
         <v>33</v>
       </c>
       <c r="T35">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC35" t="b">
         <v>0</v>
@@ -13901,7 +14063,7 @@
         <v>37</v>
       </c>
       <c r="P36" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q36">
         <v>60</v>
@@ -13913,7 +14075,7 @@
         <v>34</v>
       </c>
       <c r="T36">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W36" t="s">
         <v>266</v>
@@ -14036,7 +14198,7 @@
         <v>37</v>
       </c>
       <c r="P39" t="s">
-        <v>38</v>
+        <v>297</v>
       </c>
       <c r="Q39">
         <v>20</v>
@@ -14048,7 +14210,7 @@
         <v>0</v>
       </c>
       <c r="T39">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC39" t="b">
         <v>0</v>
@@ -14125,7 +14287,7 @@
         <v>37</v>
       </c>
       <c r="P40" t="s">
-        <v>38</v>
+        <v>301</v>
       </c>
       <c r="Q40">
         <v>20</v>
@@ -14137,7 +14299,7 @@
         <v>1</v>
       </c>
       <c r="T40">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y40" t="s">
         <v>273</v>
@@ -14214,7 +14376,7 @@
         <v>37</v>
       </c>
       <c r="P41" t="s">
-        <v>38</v>
+        <v>301</v>
       </c>
       <c r="Q41">
         <v>20</v>
@@ -14226,7 +14388,7 @@
         <v>2</v>
       </c>
       <c r="T41">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y41" t="s">
         <v>273</v>
@@ -14324,7 +14486,7 @@
         <v>37</v>
       </c>
       <c r="P42" t="s">
-        <v>38</v>
+        <v>301</v>
       </c>
       <c r="Q42">
         <v>20</v>
@@ -14336,7 +14498,7 @@
         <v>3</v>
       </c>
       <c r="T42">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y42" t="s">
         <v>273</v>
@@ -14434,7 +14596,7 @@
         <v>37</v>
       </c>
       <c r="P43" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q43">
         <v>20</v>
@@ -14523,7 +14685,7 @@
         <v>37</v>
       </c>
       <c r="P44" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q44">
         <v>20</v>
@@ -14609,7 +14771,7 @@
         <v>37</v>
       </c>
       <c r="P45" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q45">
         <v>20</v>
@@ -14691,7 +14853,7 @@
         <v>37</v>
       </c>
       <c r="P46" t="s">
-        <v>38</v>
+        <v>299</v>
       </c>
       <c r="Q46">
         <v>20</v>
@@ -14703,7 +14865,7 @@
         <v>7</v>
       </c>
       <c r="T46">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC46" t="b">
         <v>0</v>
@@ -14778,7 +14940,7 @@
         <v>37</v>
       </c>
       <c r="P47" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q47">
         <v>20</v>
@@ -14790,7 +14952,7 @@
         <v>8</v>
       </c>
       <c r="T47">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W47" t="s">
         <v>265</v>
@@ -14913,7 +15075,7 @@
         <v>37</v>
       </c>
       <c r="P50" t="s">
-        <v>38</v>
+        <v>297</v>
       </c>
       <c r="Q50">
         <v>20</v>
@@ -14925,7 +15087,7 @@
         <v>10</v>
       </c>
       <c r="T50">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC50" t="b">
         <v>0</v>
@@ -15002,7 +15164,7 @@
         <v>37</v>
       </c>
       <c r="P51" t="s">
-        <v>38</v>
+        <v>301</v>
       </c>
       <c r="Q51">
         <v>20</v>
@@ -15014,7 +15176,7 @@
         <v>11</v>
       </c>
       <c r="T51">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y51" t="s">
         <v>273</v>
@@ -15091,7 +15253,7 @@
         <v>37</v>
       </c>
       <c r="P52" t="s">
-        <v>38</v>
+        <v>301</v>
       </c>
       <c r="Q52">
         <v>20</v>
@@ -15103,7 +15265,7 @@
         <v>12</v>
       </c>
       <c r="T52">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y52" t="s">
         <v>273</v>
@@ -15201,7 +15363,7 @@
         <v>37</v>
       </c>
       <c r="P53" t="s">
-        <v>38</v>
+        <v>301</v>
       </c>
       <c r="Q53">
         <v>20</v>
@@ -15213,7 +15375,7 @@
         <v>13</v>
       </c>
       <c r="T53">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y53" t="s">
         <v>273</v>
@@ -15311,7 +15473,7 @@
         <v>37</v>
       </c>
       <c r="P54" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q54">
         <v>20</v>
@@ -15400,7 +15562,7 @@
         <v>37</v>
       </c>
       <c r="P55" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q55">
         <v>20</v>
@@ -15486,7 +15648,7 @@
         <v>37</v>
       </c>
       <c r="P56" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q56">
         <v>20</v>
@@ -15568,7 +15730,7 @@
         <v>37</v>
       </c>
       <c r="P57" t="s">
-        <v>38</v>
+        <v>299</v>
       </c>
       <c r="Q57">
         <v>20</v>
@@ -15580,7 +15742,7 @@
         <v>17</v>
       </c>
       <c r="T57">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC57" t="b">
         <v>0</v>
@@ -15655,7 +15817,7 @@
         <v>37</v>
       </c>
       <c r="P58" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q58">
         <v>20</v>
@@ -15667,7 +15829,7 @@
         <v>18</v>
       </c>
       <c r="T58">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W58" t="s">
         <v>266</v>
@@ -15790,7 +15952,7 @@
         <v>37</v>
       </c>
       <c r="P61" t="s">
-        <v>38</v>
+        <v>298</v>
       </c>
       <c r="Q61">
         <v>20</v>
@@ -15802,7 +15964,7 @@
         <v>20</v>
       </c>
       <c r="T61">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y61" t="s">
         <v>274</v>
@@ -15885,7 +16047,7 @@
         <v>37</v>
       </c>
       <c r="P62" t="s">
-        <v>38</v>
+        <v>306</v>
       </c>
       <c r="Q62">
         <v>20</v>
@@ -15897,7 +16059,7 @@
         <v>21</v>
       </c>
       <c r="T62">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y62" t="s">
         <v>274</v>
@@ -15977,7 +16139,7 @@
         <v>37</v>
       </c>
       <c r="P63" t="s">
-        <v>38</v>
+        <v>306</v>
       </c>
       <c r="Q63">
         <v>20</v>
@@ -15989,7 +16151,7 @@
         <v>22</v>
       </c>
       <c r="T63">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y63" t="s">
         <v>274</v>
@@ -16087,7 +16249,7 @@
         <v>37</v>
       </c>
       <c r="P64" t="s">
-        <v>38</v>
+        <v>306</v>
       </c>
       <c r="Q64">
         <v>20</v>
@@ -16099,7 +16261,7 @@
         <v>23</v>
       </c>
       <c r="T64">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y64" t="s">
         <v>274</v>
@@ -16197,7 +16359,7 @@
         <v>37</v>
       </c>
       <c r="P65" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q65">
         <v>20</v>
@@ -16286,7 +16448,7 @@
         <v>37</v>
       </c>
       <c r="P66" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q66">
         <v>20</v>
@@ -16372,7 +16534,7 @@
         <v>37</v>
       </c>
       <c r="P67" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q67">
         <v>20</v>
@@ -16454,7 +16616,7 @@
         <v>37</v>
       </c>
       <c r="P68" t="s">
-        <v>38</v>
+        <v>307</v>
       </c>
       <c r="Q68">
         <v>20</v>
@@ -16466,7 +16628,7 @@
         <v>27</v>
       </c>
       <c r="T68">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC68" t="b">
         <v>0</v>
@@ -16541,7 +16703,7 @@
         <v>37</v>
       </c>
       <c r="P69" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q69">
         <v>20</v>
@@ -16553,7 +16715,7 @@
         <v>28</v>
       </c>
       <c r="T69">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W69" t="s">
         <v>265</v>
@@ -16676,7 +16838,7 @@
         <v>37</v>
       </c>
       <c r="P72" t="s">
-        <v>38</v>
+        <v>298</v>
       </c>
       <c r="Q72">
         <v>20</v>
@@ -16688,7 +16850,7 @@
         <v>30</v>
       </c>
       <c r="T72">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y72" t="s">
         <v>274</v>
@@ -16771,7 +16933,7 @@
         <v>37</v>
       </c>
       <c r="P73" t="s">
-        <v>38</v>
+        <v>306</v>
       </c>
       <c r="Q73">
         <v>20</v>
@@ -16783,7 +16945,7 @@
         <v>31</v>
       </c>
       <c r="T73">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y73" t="s">
         <v>274</v>
@@ -16863,7 +17025,7 @@
         <v>37</v>
       </c>
       <c r="P74" t="s">
-        <v>38</v>
+        <v>306</v>
       </c>
       <c r="Q74">
         <v>20</v>
@@ -16875,7 +17037,7 @@
         <v>32</v>
       </c>
       <c r="T74">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y74" t="s">
         <v>274</v>
@@ -16973,7 +17135,7 @@
         <v>37</v>
       </c>
       <c r="P75" t="s">
-        <v>38</v>
+        <v>306</v>
       </c>
       <c r="Q75">
         <v>20</v>
@@ -16985,7 +17147,7 @@
         <v>33</v>
       </c>
       <c r="T75">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y75" t="s">
         <v>274</v>
@@ -17083,7 +17245,7 @@
         <v>37</v>
       </c>
       <c r="P76" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q76">
         <v>20</v>
@@ -17172,7 +17334,7 @@
         <v>37</v>
       </c>
       <c r="P77" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q77">
         <v>20</v>
@@ -17258,7 +17420,7 @@
         <v>37</v>
       </c>
       <c r="P78" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q78">
         <v>20</v>
@@ -17340,7 +17502,7 @@
         <v>37</v>
       </c>
       <c r="P79" t="s">
-        <v>38</v>
+        <v>307</v>
       </c>
       <c r="Q79">
         <v>20</v>
@@ -17352,7 +17514,7 @@
         <v>37</v>
       </c>
       <c r="T79">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC79" t="b">
         <v>0</v>
@@ -17427,7 +17589,7 @@
         <v>37</v>
       </c>
       <c r="P80" t="s">
-        <v>38</v>
+        <v>302</v>
       </c>
       <c r="Q80">
         <v>20</v>
@@ -17439,7 +17601,7 @@
         <v>38</v>
       </c>
       <c r="T80">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W80" t="s">
         <v>266</v>
@@ -17559,7 +17721,7 @@
         <v>37</v>
       </c>
       <c r="P83" t="s">
-        <v>38</v>
+        <v>306</v>
       </c>
       <c r="Q83">
         <v>20</v>
@@ -17571,7 +17733,7 @@
         <v>40</v>
       </c>
       <c r="T83">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC83" t="b">
         <v>0</v>
@@ -17648,7 +17810,7 @@
         <v>37</v>
       </c>
       <c r="P84" t="s">
-        <v>38</v>
+        <v>306</v>
       </c>
       <c r="Q84">
         <v>20</v>
@@ -17660,7 +17822,7 @@
         <v>41</v>
       </c>
       <c r="T84">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC84" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
First pass at the Common module setup. SDTBEGIN is going to need rework, probably.
</commit_message>
<xml_diff>
--- a/lighterFluid/inputs/lnlArrayMasterSheet.xlsx
+++ b/lighterFluid/inputs/lnlArrayMasterSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adambyrn\source\repos\lighterFluid\lighterFluid\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFE5CE7-40A8-479F-BD33-0654DFF313D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F110E7-FE3B-4885-99E2-0F4204088F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6434" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6434" uniqueCount="441">
   <si>
     <t>Flow</t>
   </si>
@@ -1367,6 +1367,9 @@
   <si>
     <t>COMBINE_UF_REPAIRDFF_FDS</t>
   </si>
+  <si>
+    <t>RESET1</t>
+  </si>
 </sst>
 </file>
 
@@ -43640,8 +43643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F6E2B4-C277-4E27-8556-F36877EC29FC}">
   <dimension ref="A1:AN21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="AE23" sqref="AE23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43925,39 +43928,39 @@
       </c>
       <c r="AE4" s="6" t="str">
         <f>D5</f>
-        <v>XSA_COMMON_REPAIR_E_BEGIN_T_X_X_X_RESET</v>
+        <v>XSA_COMMON_REPAIR_E_BEGIN_T_X_X_X_RESET1</v>
       </c>
       <c r="AF4" s="6" t="str">
         <f>$D18</f>
-        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET</v>
+        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET1</v>
       </c>
       <c r="AG4" s="6" t="str">
         <f t="shared" ref="AG4:AI5" si="2">$D18</f>
-        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET</v>
+        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET1</v>
       </c>
       <c r="AH4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET</v>
+        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET1</v>
       </c>
       <c r="AI4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET</v>
+        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET1</v>
       </c>
       <c r="AJ4" s="6" t="str">
         <f>D5</f>
-        <v>XSA_COMMON_REPAIR_E_BEGIN_T_X_X_X_RESET</v>
+        <v>XSA_COMMON_REPAIR_E_BEGIN_T_X_X_X_RESET1</v>
       </c>
       <c r="AK4" s="6" t="str">
         <f>D5</f>
-        <v>XSA_COMMON_REPAIR_E_BEGIN_T_X_X_X_RESET</v>
+        <v>XSA_COMMON_REPAIR_E_BEGIN_T_X_X_X_RESET1</v>
       </c>
       <c r="AL4" s="6" t="str">
         <f>D5</f>
-        <v>XSA_COMMON_REPAIR_E_BEGIN_T_X_X_X_RESET</v>
+        <v>XSA_COMMON_REPAIR_E_BEGIN_T_X_X_X_RESET1</v>
       </c>
       <c r="AM4" s="6" t="str">
         <f>D5</f>
-        <v>XSA_COMMON_REPAIR_E_BEGIN_T_X_X_X_RESET</v>
+        <v>XSA_COMMON_REPAIR_E_BEGIN_T_X_X_X_RESET1</v>
       </c>
       <c r="AN4" s="6"/>
     </row>
@@ -43974,7 +43977,7 @@
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>XSA_COMMON_REPAIR_E_BEGIN_T_X_X_X_RESET</v>
+        <v>XSA_COMMON_REPAIR_E_BEGIN_T_X_X_X_RESET1</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>386</v>
@@ -44001,7 +44004,7 @@
         <v>6</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>434</v>
+        <v>440</v>
       </c>
       <c r="N5" s="6" t="s">
         <v>36</v>
@@ -44929,39 +44932,39 @@
       </c>
       <c r="AE17" s="21" t="str">
         <f>D18</f>
-        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET</v>
+        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET1</v>
       </c>
       <c r="AF17" s="21" t="str">
         <f>$D18</f>
-        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET</v>
+        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET1</v>
       </c>
       <c r="AG17" s="21" t="str">
         <f t="shared" ref="AG17:AI17" si="13">$D18</f>
-        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET</v>
+        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET1</v>
       </c>
       <c r="AH17" s="21" t="str">
         <f t="shared" si="13"/>
-        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET</v>
+        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET1</v>
       </c>
       <c r="AI17" s="21" t="str">
         <f t="shared" si="13"/>
-        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET</v>
+        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET1</v>
       </c>
       <c r="AJ17" s="21" t="str">
         <f>D18</f>
-        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET</v>
+        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET1</v>
       </c>
       <c r="AK17" s="21" t="str">
         <f>D18</f>
-        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET</v>
+        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET1</v>
       </c>
       <c r="AL17" s="21" t="str">
         <f>D18</f>
-        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET</v>
+        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET1</v>
       </c>
       <c r="AM17" s="21" t="str">
         <f>D18</f>
-        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET</v>
+        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET1</v>
       </c>
     </row>
     <row r="18" spans="1:40" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -44977,7 +44980,7 @@
       </c>
       <c r="D18" s="21" t="str">
         <f t="shared" si="11"/>
-        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET</v>
+        <v>XSA_COMMON_REPAIR_E_SDTBEGIN_T_X_X_X_RESET1</v>
       </c>
       <c r="E18" s="21" t="s">
         <v>386</v>
@@ -45004,7 +45007,7 @@
         <v>6</v>
       </c>
       <c r="M18" s="21" t="s">
-        <v>434</v>
+        <v>440</v>
       </c>
       <c r="N18" s="21" t="s">
         <v>36</v>

</xml_diff>